<commit_message>
Updated to latest ISO4217 standard.
Added South Sudanese Pound.

Closes #1.
</commit_message>
<xml_diff>
--- a/src/CodeFragments.MoneyAndCurrency/Currencies/CurrencyList.xlsx
+++ b/src/CodeFragments.MoneyAndCurrency/Currencies/CurrencyList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="22980" windowHeight="10845"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="22980" windowHeight="10848"/>
   </bookViews>
   <sheets>
     <sheet name="ISO 4217" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="671">
   <si>
     <t>Afghani</t>
   </si>
@@ -2021,13 +2021,19 @@
   </si>
   <si>
     <t>Initialization</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>South Sudanese Pound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2047,6 +2053,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2081,7 +2092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2094,6 +2105,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2388,28 +2400,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J181"/>
+  <dimension ref="A1:J182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I157" sqref="I157"/>
+      <selection pane="bottomRight" activeCell="J137" sqref="J137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="77.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="3"/>
+    <col min="9" max="9" width="44.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="82.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="7" customFormat="1">
@@ -2449,7 +2461,7 @@
         <v>292</v>
       </c>
       <c r="B2" s="2">
-        <v>784</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>291</v>
@@ -2469,13 +2481,13 @@
       <c r="H2" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="I2" s="3" t="str">
+      <c r="I2" s="8" t="str">
         <f>CONCATENATE("public static Currency ", A2, " { get; private set; }")</f>
         <v>public static Currency AED { get; private set; }</v>
       </c>
-      <c r="J2" s="3" t="str">
-        <f>CONCATENATE("{", A2, " = new Currency(""",A2,""", ", B2,", """, C2,""", ",G2, ")},")</f>
-        <v>{AED = new Currency("AED", 784, "UAE Dirham", 2)},</v>
+      <c r="J2" s="8" t="str">
+        <f>CONCATENATE("{ ", A2, " = new Currency(""",A2,""", ", B2,", """, C2,""", ",G2, ") },")</f>
+        <v>{ AED = new Currency("AED", 1, "UAE Dirham", 2) },</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2503,13 +2515,13 @@
       <c r="H3" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="I3" s="3" t="str">
+      <c r="I3" s="8" t="str">
         <f t="shared" ref="I3:I66" si="0">CONCATENATE("public static Currency ", A3, " { get; private set; }")</f>
         <v>public static Currency AFN { get; private set; }</v>
       </c>
-      <c r="J3" s="3" t="str">
-        <f t="shared" ref="J3:J66" si="1">CONCATENATE("{", A3, " = new Currency(""",A3,""", ", B3,", """, C3,""", ",G3, ")},")</f>
-        <v>{AFN = new Currency("AFN", 971, "Afghani", 2)},</v>
+      <c r="J3" s="8" t="str">
+        <f t="shared" ref="J3:J66" si="1">CONCATENATE("{ ", A3, " = new Currency(""",A3,""", ", B3,", """, C3,""", ",G3, ") },")</f>
+        <v>{ AFN = new Currency("AFN", 971, "Afghani", 2) },</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2537,13 +2549,13 @@
       <c r="H4" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="I4" s="3" t="str">
+      <c r="I4" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency ALL { get; private set; }</v>
       </c>
-      <c r="J4" s="3" t="str">
+      <c r="J4" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{ALL = new Currency("ALL", 8, "Albanian Lek", 2)},</v>
+        <v>{ ALL = new Currency("ALL", 8, "Albanian Lek", 2) },</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2568,13 +2580,13 @@
       <c r="G5" s="3">
         <v>2</v>
       </c>
-      <c r="I5" s="3" t="str">
+      <c r="I5" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency AMD { get; private set; }</v>
       </c>
-      <c r="J5" s="3" t="str">
+      <c r="J5" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{AMD = new Currency("AMD", 51, "Armenian Dram", 2)},</v>
+        <v>{ AMD = new Currency("AMD", 51, "Armenian Dram", 2) },</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2602,13 +2614,13 @@
       <c r="H6" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="I6" s="3" t="str">
+      <c r="I6" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency ANG { get; private set; }</v>
       </c>
-      <c r="J6" s="3" t="str">
+      <c r="J6" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{ANG = new Currency("ANG", 532, "Netherlands Antillean Guilder", 2)},</v>
+        <v>{ ANG = new Currency("ANG", 532, "Netherlands Antillean Guilder", 2) },</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2636,13 +2648,13 @@
       <c r="H7" s="3" t="s">
         <v>608</v>
       </c>
-      <c r="I7" s="3" t="str">
+      <c r="I7" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency AOA { get; private set; }</v>
       </c>
-      <c r="J7" s="3" t="str">
+      <c r="J7" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{AOA = new Currency("AOA", 973, "Angolan Kwanza", 2)},</v>
+        <v>{ AOA = new Currency("AOA", 973, "Angolan Kwanza", 2) },</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2670,13 +2682,13 @@
       <c r="H8" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="I8" s="3" t="str">
+      <c r="I8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency ARS { get; private set; }</v>
       </c>
-      <c r="J8" s="3" t="str">
+      <c r="J8" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{ARS = new Currency("ARS", 32, "Argentine Peso", 2)},</v>
+        <v>{ ARS = new Currency("ARS", 32, "Argentine Peso", 2) },</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2704,13 +2716,13 @@
       <c r="H9" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="I9" s="3" t="str">
+      <c r="I9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency AUD { get; private set; }</v>
       </c>
-      <c r="J9" s="3" t="str">
+      <c r="J9" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{AUD = new Currency("AUD", 36, "Australian Dollar", 2)},</v>
+        <v>{ AUD = new Currency("AUD", 36, "Australian Dollar", 2) },</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2738,13 +2750,13 @@
       <c r="H10" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="I10" s="3" t="str">
+      <c r="I10" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency AWG { get; private set; }</v>
       </c>
-      <c r="J10" s="3" t="str">
+      <c r="J10" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{AWG = new Currency("AWG", 533, "Aruban Florin", 2)},</v>
+        <v>{ AWG = new Currency("AWG", 533, "Aruban Florin", 2) },</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2772,13 +2784,13 @@
       <c r="H11" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="I11" s="3" t="str">
+      <c r="I11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency AZN { get; private set; }</v>
       </c>
-      <c r="J11" s="3" t="str">
+      <c r="J11" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{AZN = new Currency("AZN", 944, "Azerbaijanian Manat", 2)},</v>
+        <v>{ AZN = new Currency("AZN", 944, "Azerbaijanian Manat", 2) },</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2806,13 +2818,13 @@
       <c r="H12" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="I12" s="3" t="str">
+      <c r="I12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BAM { get; private set; }</v>
       </c>
-      <c r="J12" s="3" t="str">
+      <c r="J12" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BAM = new Currency("BAM", 977, "Bosnia And Herzegovina Convertible Mark", 2)},</v>
+        <v>{ BAM = new Currency("BAM", 977, "Bosnia And Herzegovina Convertible Mark", 2) },</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2840,13 +2852,13 @@
       <c r="H13" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="I13" s="3" t="str">
+      <c r="I13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BBD { get; private set; }</v>
       </c>
-      <c r="J13" s="3" t="str">
+      <c r="J13" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BBD = new Currency("BBD", 52, "Barbados Dollar", 2)},</v>
+        <v>{ BBD = new Currency("BBD", 52, "Barbados Dollar", 2) },</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2874,13 +2886,13 @@
       <c r="H14" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="I14" s="3" t="str">
+      <c r="I14" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BDT { get; private set; }</v>
       </c>
-      <c r="J14" s="3" t="str">
+      <c r="J14" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BDT = new Currency("BDT", 50, "Bangladeshi Taka", 2)},</v>
+        <v>{ BDT = new Currency("BDT", 50, "Bangladeshi Taka", 2) },</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2908,13 +2920,13 @@
       <c r="H15" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="I15" s="3" t="str">
+      <c r="I15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BGN { get; private set; }</v>
       </c>
-      <c r="J15" s="3" t="str">
+      <c r="J15" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BGN = new Currency("BGN", 975, "Bulgarian Lev", 2)},</v>
+        <v>{ BGN = new Currency("BGN", 975, "Bulgarian Lev", 2) },</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2942,13 +2954,13 @@
       <c r="H16" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="I16" s="3" t="str">
+      <c r="I16" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BHD { get; private set; }</v>
       </c>
-      <c r="J16" s="3" t="str">
+      <c r="J16" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BHD = new Currency("BHD", 48, "Bahraini Dinar", 3)},</v>
+        <v>{ BHD = new Currency("BHD", 48, "Bahraini Dinar", 3) },</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2976,13 +2988,13 @@
       <c r="H17" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="I17" s="3" t="str">
+      <c r="I17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BIF { get; private set; }</v>
       </c>
-      <c r="J17" s="3" t="str">
+      <c r="J17" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BIF = new Currency("BIF", 108, "Burundi Franc", 0)},</v>
+        <v>{ BIF = new Currency("BIF", 108, "Burundi Franc", 0) },</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3010,13 +3022,13 @@
       <c r="H18" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="I18" s="3" t="str">
+      <c r="I18" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BMD { get; private set; }</v>
       </c>
-      <c r="J18" s="3" t="str">
+      <c r="J18" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BMD = new Currency("BMD", 60, "Bermudian Dollar", 2)},</v>
+        <v>{ BMD = new Currency("BMD", 60, "Bermudian Dollar", 2) },</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3044,13 +3056,13 @@
       <c r="H19" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="I19" s="3" t="str">
+      <c r="I19" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BND { get; private set; }</v>
       </c>
-      <c r="J19" s="3" t="str">
+      <c r="J19" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BND = new Currency("BND", 96, "Brunei Dollar", 2)},</v>
+        <v>{ BND = new Currency("BND", 96, "Brunei Dollar", 2) },</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3078,13 +3090,13 @@
       <c r="H20" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="I20" s="3" t="str">
+      <c r="I20" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BOB { get; private set; }</v>
       </c>
-      <c r="J20" s="3" t="str">
+      <c r="J20" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BOB = new Currency("BOB", 68, "Boliviano", 2)},</v>
+        <v>{ BOB = new Currency("BOB", 68, "Boliviano", 2) },</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3103,13 +3115,13 @@
       <c r="G21" s="3">
         <v>0</v>
       </c>
-      <c r="I21" s="3" t="str">
+      <c r="I21" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BOV { get; private set; }</v>
       </c>
-      <c r="J21" s="3" t="str">
+      <c r="J21" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BOV = new Currency("BOV", 984, "Bolivian Mvdol (funds code)", 0)},</v>
+        <v>{ BOV = new Currency("BOV", 984, "Bolivian Mvdol (funds code)", 0) },</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -3137,13 +3149,13 @@
       <c r="H22" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="I22" s="3" t="str">
+      <c r="I22" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BRL { get; private set; }</v>
       </c>
-      <c r="J22" s="3" t="str">
+      <c r="J22" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BRL = new Currency("BRL", 986, "Brazilian Real", 2)},</v>
+        <v>{ BRL = new Currency("BRL", 986, "Brazilian Real", 2) },</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -3171,13 +3183,13 @@
       <c r="H23" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="I23" s="3" t="str">
+      <c r="I23" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BSD { get; private set; }</v>
       </c>
-      <c r="J23" s="3" t="str">
+      <c r="J23" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BSD = new Currency("BSD", 44, "Bahamian Dollar", 2)},</v>
+        <v>{ BSD = new Currency("BSD", 44, "Bahamian Dollar", 2) },</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3205,13 +3217,13 @@
       <c r="H24" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="I24" s="3" t="str">
+      <c r="I24" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BTN { get; private set; }</v>
       </c>
-      <c r="J24" s="3" t="str">
+      <c r="J24" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BTN = new Currency("BTN", 64, "Bhutanese Ngultrum", 2)},</v>
+        <v>{ BTN = new Currency("BTN", 64, "Bhutanese Ngultrum", 2) },</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -3239,13 +3251,13 @@
       <c r="H25" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="I25" s="3" t="str">
+      <c r="I25" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BWP { get; private set; }</v>
       </c>
-      <c r="J25" s="3" t="str">
+      <c r="J25" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BWP = new Currency("BWP", 72, "Botswana Pula", 2)},</v>
+        <v>{ BWP = new Currency("BWP", 72, "Botswana Pula", 2) },</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -3273,13 +3285,13 @@
       <c r="H26" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="I26" s="3" t="str">
+      <c r="I26" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BYR { get; private set; }</v>
       </c>
-      <c r="J26" s="3" t="str">
+      <c r="J26" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BYR = new Currency("BYR", 974, "Belarusian Ruble", 0)},</v>
+        <v>{ BYR = new Currency("BYR", 974, "Belarusian Ruble", 0) },</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -3307,13 +3319,13 @@
       <c r="H27" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="I27" s="3" t="str">
+      <c r="I27" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency BZD { get; private set; }</v>
       </c>
-      <c r="J27" s="3" t="str">
+      <c r="J27" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{BZD = new Currency("BZD", 84, "Belize Dollar", 2)},</v>
+        <v>{ BZD = new Currency("BZD", 84, "Belize Dollar", 2) },</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -3341,13 +3353,13 @@
       <c r="H28" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="I28" s="3" t="str">
+      <c r="I28" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CAD { get; private set; }</v>
       </c>
-      <c r="J28" s="3" t="str">
+      <c r="J28" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CAD = new Currency("CAD", 124, "Canadian Dollar", 2)},</v>
+        <v>{ CAD = new Currency("CAD", 124, "Canadian Dollar", 2) },</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -3375,13 +3387,13 @@
       <c r="H29" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="I29" s="3" t="str">
+      <c r="I29" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CDF { get; private set; }</v>
       </c>
-      <c r="J29" s="3" t="str">
+      <c r="J29" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CDF = new Currency("CDF", 976, "Congolese Franc", 0)},</v>
+        <v>{ CDF = new Currency("CDF", 976, "Congolese Franc", 0) },</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -3406,13 +3418,13 @@
       <c r="G30" s="3">
         <v>2</v>
       </c>
-      <c r="I30" s="3" t="str">
+      <c r="I30" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CHE { get; private set; }</v>
       </c>
-      <c r="J30" s="3" t="str">
+      <c r="J30" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CHE = new Currency("CHE", 947, "WIR Euro", 2)},</v>
+        <v>{ CHE = new Currency("CHE", 947, "WIR Euro", 2) },</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -3440,13 +3452,13 @@
       <c r="H31" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="I31" s="3" t="str">
+      <c r="I31" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CHF { get; private set; }</v>
       </c>
-      <c r="J31" s="3" t="str">
+      <c r="J31" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CHF = new Currency("CHF", 756, "Swiss Franc", 2)},</v>
+        <v>{ CHF = new Currency("CHF", 756, "Swiss Franc", 2) },</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -3471,13 +3483,13 @@
       <c r="G32" s="3">
         <v>2</v>
       </c>
-      <c r="I32" s="3" t="str">
+      <c r="I32" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CHW { get; private set; }</v>
       </c>
-      <c r="J32" s="3" t="str">
+      <c r="J32" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CHW = new Currency("CHW", 948, "WIR Franc", 2)},</v>
+        <v>{ CHW = new Currency("CHW", 948, "WIR Franc", 2) },</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -3499,13 +3511,13 @@
       <c r="H33" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="I33" s="3" t="str">
+      <c r="I33" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CLF { get; private set; }</v>
       </c>
-      <c r="J33" s="3" t="str">
+      <c r="J33" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CLF = new Currency("CLF", 990, "Unidad de Fomento", 0)},</v>
+        <v>{ CLF = new Currency("CLF", 990, "Unidad de Fomento", 0) },</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3533,13 +3545,13 @@
       <c r="H34" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="I34" s="3" t="str">
+      <c r="I34" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CLP { get; private set; }</v>
       </c>
-      <c r="J34" s="3" t="str">
+      <c r="J34" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CLP = new Currency("CLP", 152, "Chilean Peso", 0)},</v>
+        <v>{ CLP = new Currency("CLP", 152, "Chilean Peso", 0) },</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3567,13 +3579,13 @@
       <c r="H35" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="I35" s="3" t="str">
+      <c r="I35" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CNY { get; private set; }</v>
       </c>
-      <c r="J35" s="3" t="str">
+      <c r="J35" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CNY = new Currency("CNY", 156, "Yuan Renminbi", 2)},</v>
+        <v>{ CNY = new Currency("CNY", 156, "Yuan Renminbi", 2) },</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -3601,13 +3613,13 @@
       <c r="H36" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="I36" s="3" t="str">
+      <c r="I36" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency COP { get; private set; }</v>
       </c>
-      <c r="J36" s="3" t="str">
+      <c r="J36" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{COP = new Currency("COP", 170, "Colombian Peso", 2)},</v>
+        <v>{ COP = new Currency("COP", 170, "Colombian Peso", 2) },</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -3626,13 +3638,13 @@
       <c r="G37" s="3">
         <v>2</v>
       </c>
-      <c r="I37" s="3" t="str">
+      <c r="I37" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency COU { get; private set; }</v>
       </c>
-      <c r="J37" s="3" t="str">
+      <c r="J37" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{COU = new Currency("COU", 970, "Unidad de Valor Real", 2)},</v>
+        <v>{ COU = new Currency("COU", 970, "Unidad de Valor Real", 2) },</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -3660,13 +3672,13 @@
       <c r="H38" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="I38" s="3" t="str">
+      <c r="I38" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CRC { get; private set; }</v>
       </c>
-      <c r="J38" s="3" t="str">
+      <c r="J38" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CRC = new Currency("CRC", 188, "Costa Rican Colón", 2)},</v>
+        <v>{ CRC = new Currency("CRC", 188, "Costa Rican Colón", 2) },</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -3694,13 +3706,13 @@
       <c r="H39" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="I39" s="3" t="str">
+      <c r="I39" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CUC { get; private set; }</v>
       </c>
-      <c r="J39" s="3" t="str">
+      <c r="J39" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CUC = new Currency("CUC", 931, "Cuban Convertible Peso", 2)},</v>
+        <v>{ CUC = new Currency("CUC", 931, "Cuban Convertible Peso", 2) },</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -3728,13 +3740,13 @@
       <c r="H40" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="I40" s="3" t="str">
+      <c r="I40" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CUP { get; private set; }</v>
       </c>
-      <c r="J40" s="3" t="str">
+      <c r="J40" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CUP = new Currency("CUP", 192, "Cuban Peso", 2)},</v>
+        <v>{ CUP = new Currency("CUP", 192, "Cuban Peso", 2) },</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -3762,13 +3774,13 @@
       <c r="H41" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="I41" s="3" t="str">
+      <c r="I41" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CVE { get; private set; }</v>
       </c>
-      <c r="J41" s="3" t="str">
+      <c r="J41" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CVE = new Currency("CVE", 132, "Cape Verde Escudo", 2)},</v>
+        <v>{ CVE = new Currency("CVE", 132, "Cape Verde Escudo", 2) },</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -3796,13 +3808,13 @@
       <c r="H42" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="I42" s="3" t="str">
+      <c r="I42" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency CZK { get; private set; }</v>
       </c>
-      <c r="J42" s="3" t="str">
+      <c r="J42" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{CZK = new Currency("CZK", 203, "Czech Koruna", 2)},</v>
+        <v>{ CZK = new Currency("CZK", 203, "Czech Koruna", 2) },</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -3830,13 +3842,13 @@
       <c r="H43" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="I43" s="3" t="str">
+      <c r="I43" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency DJF { get; private set; }</v>
       </c>
-      <c r="J43" s="3" t="str">
+      <c r="J43" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{DJF = new Currency("DJF", 262, "Djibouti Franc", 2)},</v>
+        <v>{ DJF = new Currency("DJF", 262, "Djibouti Franc", 2) },</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -3864,13 +3876,13 @@
       <c r="H44" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="I44" s="3" t="str">
+      <c r="I44" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency DKK { get; private set; }</v>
       </c>
-      <c r="J44" s="3" t="str">
+      <c r="J44" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{DKK = new Currency("DKK", 208, "Danish Krone", 2)},</v>
+        <v>{ DKK = new Currency("DKK", 208, "Danish Krone", 2) },</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -3898,13 +3910,13 @@
       <c r="H45" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="I45" s="3" t="str">
+      <c r="I45" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency DOP { get; private set; }</v>
       </c>
-      <c r="J45" s="3" t="str">
+      <c r="J45" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{DOP = new Currency("DOP", 214, "Dominican Peso", 2)},</v>
+        <v>{ DOP = new Currency("DOP", 214, "Dominican Peso", 2) },</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -3932,13 +3944,13 @@
       <c r="H46" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="I46" s="3" t="str">
+      <c r="I46" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency DZD { get; private set; }</v>
       </c>
-      <c r="J46" s="3" t="str">
+      <c r="J46" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{DZD = new Currency("DZD", 12, "Algerian Dinar", 2)},</v>
+        <v>{ DZD = new Currency("DZD", 12, "Algerian Dinar", 2) },</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -3966,13 +3978,13 @@
       <c r="H47" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="I47" s="3" t="str">
+      <c r="I47" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency EEK { get; private set; }</v>
       </c>
-      <c r="J47" s="3" t="str">
+      <c r="J47" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{EEK = new Currency("EEK", 233, "Estonian Kroon", 2)},</v>
+        <v>{ EEK = new Currency("EEK", 233, "Estonian Kroon", 2) },</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -4000,13 +4012,13 @@
       <c r="H48" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="I48" s="3" t="str">
+      <c r="I48" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency EGP { get; private set; }</v>
       </c>
-      <c r="J48" s="3" t="str">
+      <c r="J48" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{EGP = new Currency("EGP", 818, "Egyptian Pound", 2)},</v>
+        <v>{ EGP = new Currency("EGP", 818, "Egyptian Pound", 2) },</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -4034,13 +4046,13 @@
       <c r="H49" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="I49" s="3" t="str">
+      <c r="I49" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency ERN { get; private set; }</v>
       </c>
-      <c r="J49" s="3" t="str">
+      <c r="J49" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{ERN = new Currency("ERN", 232, "Eritrean Nakfa", 0)},</v>
+        <v>{ ERN = new Currency("ERN", 232, "Eritrean Nakfa", 0) },</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -4068,13 +4080,13 @@
       <c r="H50" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="I50" s="3" t="str">
+      <c r="I50" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency ETB { get; private set; }</v>
       </c>
-      <c r="J50" s="3" t="str">
+      <c r="J50" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{ETB = new Currency("ETB", 230, "Ethiopian Birr", 2)},</v>
+        <v>{ ETB = new Currency("ETB", 230, "Ethiopian Birr", 2) },</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -4102,13 +4114,13 @@
       <c r="H51" s="3" t="s">
         <v>636</v>
       </c>
-      <c r="I51" s="3" t="str">
+      <c r="I51" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency EUR { get; private set; }</v>
       </c>
-      <c r="J51" s="3" t="str">
+      <c r="J51" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{EUR = new Currency("EUR", 978, "Euro", 2)},</v>
+        <v>{ EUR = new Currency("EUR", 978, "Euro", 2) },</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -4136,13 +4148,13 @@
       <c r="H52" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="I52" s="3" t="str">
+      <c r="I52" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency FJD { get; private set; }</v>
       </c>
-      <c r="J52" s="3" t="str">
+      <c r="J52" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{FJD = new Currency("FJD", 242, "Fiji Dollar", 2)},</v>
+        <v>{ FJD = new Currency("FJD", 242, "Fiji Dollar", 2) },</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -4170,13 +4182,13 @@
       <c r="H53" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="I53" s="3" t="str">
+      <c r="I53" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency FKP { get; private set; }</v>
       </c>
-      <c r="J53" s="3" t="str">
+      <c r="J53" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{FKP = new Currency("FKP", 238, "Falkland Islands Pound", 2)},</v>
+        <v>{ FKP = new Currency("FKP", 238, "Falkland Islands Pound", 2) },</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -4204,13 +4216,13 @@
       <c r="H54" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I54" s="3" t="str">
+      <c r="I54" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency GBP { get; private set; }</v>
       </c>
-      <c r="J54" s="3" t="str">
+      <c r="J54" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{GBP = new Currency("GBP", 826, "Pound Sterling", 2)},</v>
+        <v>{ GBP = new Currency("GBP", 826, "Pound Sterling", 2) },</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -4235,13 +4247,13 @@
       <c r="G55" s="3">
         <v>2</v>
       </c>
-      <c r="I55" s="3" t="str">
+      <c r="I55" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency GEL { get; private set; }</v>
       </c>
-      <c r="J55" s="3" t="str">
+      <c r="J55" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{GEL = new Currency("GEL", 981, "Georgian Lari", 2)},</v>
+        <v>{ GEL = new Currency("GEL", 981, "Georgian Lari", 2) },</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -4269,13 +4281,13 @@
       <c r="H56" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="I56" s="3" t="str">
+      <c r="I56" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency GHS { get; private set; }</v>
       </c>
-      <c r="J56" s="3" t="str">
+      <c r="J56" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{GHS = new Currency("GHS", 936, "Ghanaian Cedi", 2)},</v>
+        <v>{ GHS = new Currency("GHS", 936, "Ghanaian Cedi", 2) },</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -4303,13 +4315,13 @@
       <c r="H57" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I57" s="3" t="str">
+      <c r="I57" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency GIP { get; private set; }</v>
       </c>
-      <c r="J57" s="3" t="str">
+      <c r="J57" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{GIP = new Currency("GIP", 292, "Gibraltar Pound", 2)},</v>
+        <v>{ GIP = new Currency("GIP", 292, "Gibraltar Pound", 2) },</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -4337,13 +4349,13 @@
       <c r="H58" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="I58" s="3" t="str">
+      <c r="I58" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency GMD { get; private set; }</v>
       </c>
-      <c r="J58" s="3" t="str">
+      <c r="J58" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{GMD = new Currency("GMD", 270, "Gambian Dalasi", 2)},</v>
+        <v>{ GMD = new Currency("GMD", 270, "Gambian Dalasi", 2) },</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -4371,13 +4383,13 @@
       <c r="H59" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="I59" s="3" t="str">
+      <c r="I59" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency GNF { get; private set; }</v>
       </c>
-      <c r="J59" s="3" t="str">
+      <c r="J59" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{GNF = new Currency("GNF", 324, "Guinean Franc", 2)},</v>
+        <v>{ GNF = new Currency("GNF", 324, "Guinean Franc", 2) },</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -4405,13 +4417,13 @@
       <c r="H60" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="I60" s="3" t="str">
+      <c r="I60" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency GTQ { get; private set; }</v>
       </c>
-      <c r="J60" s="3" t="str">
+      <c r="J60" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{GTQ = new Currency("GTQ", 320, "Guatemalan Quetzal", 2)},</v>
+        <v>{ GTQ = new Currency("GTQ", 320, "Guatemalan Quetzal", 2) },</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -4439,13 +4451,13 @@
       <c r="H61" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="I61" s="3" t="str">
+      <c r="I61" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency GYD { get; private set; }</v>
       </c>
-      <c r="J61" s="3" t="str">
+      <c r="J61" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{GYD = new Currency("GYD", 328, "Guyana Dollar", 2)},</v>
+        <v>{ GYD = new Currency("GYD", 328, "Guyana Dollar", 2) },</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -4473,13 +4485,13 @@
       <c r="H62" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="I62" s="3" t="str">
+      <c r="I62" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency HKD { get; private set; }</v>
       </c>
-      <c r="J62" s="3" t="str">
+      <c r="J62" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{HKD = new Currency("HKD", 344, "Hong Kong Dollar", 2)},</v>
+        <v>{ HKD = new Currency("HKD", 344, "Hong Kong Dollar", 2) },</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -4507,13 +4519,13 @@
       <c r="H63" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="I63" s="3" t="str">
+      <c r="I63" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency HNL { get; private set; }</v>
       </c>
-      <c r="J63" s="3" t="str">
+      <c r="J63" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{HNL = new Currency("HNL", 340, "Honduran Lempira", 2)},</v>
+        <v>{ HNL = new Currency("HNL", 340, "Honduran Lempira", 2) },</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -4541,13 +4553,13 @@
       <c r="H64" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="I64" s="3" t="str">
+      <c r="I64" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency HRK { get; private set; }</v>
       </c>
-      <c r="J64" s="3" t="str">
+      <c r="J64" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{HRK = new Currency("HRK", 191, "Croatian Kuna", 2)},</v>
+        <v>{ HRK = new Currency("HRK", 191, "Croatian Kuna", 2) },</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -4575,13 +4587,13 @@
       <c r="H65" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="I65" s="3" t="str">
+      <c r="I65" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency HTG { get; private set; }</v>
       </c>
-      <c r="J65" s="3" t="str">
+      <c r="J65" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{HTG = new Currency("HTG", 332, "Haitian Gourde", 2)},</v>
+        <v>{ HTG = new Currency("HTG", 332, "Haitian Gourde", 2) },</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -4609,13 +4621,13 @@
       <c r="H66" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="I66" s="3" t="str">
+      <c r="I66" s="8" t="str">
         <f t="shared" si="0"/>
         <v>public static Currency HUF { get; private set; }</v>
       </c>
-      <c r="J66" s="3" t="str">
+      <c r="J66" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>{HUF = new Currency("HUF", 348, "Hungarian Forint", 0)},</v>
+        <v>{ HUF = new Currency("HUF", 348, "Hungarian Forint", 0) },</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -4643,13 +4655,13 @@
       <c r="H67" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="I67" s="3" t="str">
+      <c r="I67" s="8" t="str">
         <f t="shared" ref="I67:I130" si="2">CONCATENATE("public static Currency ", A67, " { get; private set; }")</f>
         <v>public static Currency IDR { get; private set; }</v>
       </c>
-      <c r="J67" s="3" t="str">
-        <f t="shared" ref="J67:J130" si="3">CONCATENATE("{", A67, " = new Currency(""",A67,""", ", B67,", """, C67,""", ",G67, ")},")</f>
-        <v>{IDR = new Currency("IDR", 360, "Indonesian Rupiah", 0)},</v>
+      <c r="J67" s="8" t="str">
+        <f t="shared" ref="J67:J130" si="3">CONCATENATE("{ ", A67, " = new Currency(""",A67,""", ", B67,", """, C67,""", ",G67, ") },")</f>
+        <v>{ IDR = new Currency("IDR", 360, "Indonesian Rupiah", 0) },</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -4677,13 +4689,13 @@
       <c r="H68" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="I68" s="3" t="str">
+      <c r="I68" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency ILS { get; private set; }</v>
       </c>
-      <c r="J68" s="3" t="str">
+      <c r="J68" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{ILS = new Currency("ILS", 376, "Israeli New Shekel", 2)},</v>
+        <v>{ ILS = new Currency("ILS", 376, "Israeli New Shekel", 2) },</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -4711,13 +4723,13 @@
       <c r="H69" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="I69" s="3" t="str">
+      <c r="I69" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency INR { get; private set; }</v>
       </c>
-      <c r="J69" s="3" t="str">
+      <c r="J69" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{INR = new Currency("INR", 356, "Indian Rupee", 2)},</v>
+        <v>{ INR = new Currency("INR", 356, "Indian Rupee", 2) },</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -4745,13 +4757,13 @@
       <c r="H70" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="I70" s="3" t="str">
+      <c r="I70" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency IQD { get; private set; }</v>
       </c>
-      <c r="J70" s="3" t="str">
+      <c r="J70" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{IQD = new Currency("IQD", 368, "Iraqi Dinar", 3)},</v>
+        <v>{ IQD = new Currency("IQD", 368, "Iraqi Dinar", 3) },</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -4779,13 +4791,13 @@
       <c r="H71" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="I71" s="3" t="str">
+      <c r="I71" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency IRR { get; private set; }</v>
       </c>
-      <c r="J71" s="3" t="str">
+      <c r="J71" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{IRR = new Currency("IRR", 364, "Iranian Rial", 0)},</v>
+        <v>{ IRR = new Currency("IRR", 364, "Iranian Rial", 0) },</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -4813,13 +4825,13 @@
       <c r="H72" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="I72" s="3" t="str">
+      <c r="I72" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency ISK { get; private set; }</v>
       </c>
-      <c r="J72" s="3" t="str">
+      <c r="J72" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{ISK = new Currency("ISK", 352, "Icelandic Króna", 2)},</v>
+        <v>{ ISK = new Currency("ISK", 352, "Icelandic Króna", 2) },</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -4847,13 +4859,13 @@
       <c r="H73" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="I73" s="3" t="str">
+      <c r="I73" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency JMD { get; private set; }</v>
       </c>
-      <c r="J73" s="3" t="str">
+      <c r="J73" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{JMD = new Currency("JMD", 388, "Jamaican Dollar", 2)},</v>
+        <v>{ JMD = new Currency("JMD", 388, "Jamaican Dollar", 2) },</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -4881,13 +4893,13 @@
       <c r="H74" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I74" s="3" t="str">
+      <c r="I74" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency JOD { get; private set; }</v>
       </c>
-      <c r="J74" s="3" t="str">
+      <c r="J74" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{JOD = new Currency("JOD", 400, "Jordanian Dinar", 3)},</v>
+        <v>{ JOD = new Currency("JOD", 400, "Jordanian Dinar", 3) },</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -4915,13 +4927,13 @@
       <c r="H75" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="I75" s="3" t="str">
+      <c r="I75" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency JPY { get; private set; }</v>
       </c>
-      <c r="J75" s="3" t="str">
+      <c r="J75" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{JPY = new Currency("JPY", 392, "Japanese Yen", 0)},</v>
+        <v>{ JPY = new Currency("JPY", 392, "Japanese Yen", 0) },</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -4949,13 +4961,13 @@
       <c r="H76" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="I76" s="3" t="str">
+      <c r="I76" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KES { get; private set; }</v>
       </c>
-      <c r="J76" s="3" t="str">
+      <c r="J76" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KES = new Currency("KES", 404, "Kenyan Shilling", 2)},</v>
+        <v>{ KES = new Currency("KES", 404, "Kenyan Shilling", 2) },</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -4980,13 +4992,13 @@
       <c r="G77" s="3">
         <v>0</v>
       </c>
-      <c r="I77" s="3" t="str">
+      <c r="I77" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KGS { get; private set; }</v>
       </c>
-      <c r="J77" s="3" t="str">
+      <c r="J77" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KGS = new Currency("KGS", 417, "Kyrgyzstani Som", 0)},</v>
+        <v>{ KGS = new Currency("KGS", 417, "Kyrgyzstani Som", 0) },</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -5014,13 +5026,13 @@
       <c r="H78" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="I78" s="3" t="str">
+      <c r="I78" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KHR { get; private set; }</v>
       </c>
-      <c r="J78" s="3" t="str">
+      <c r="J78" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KHR = new Currency("KHR", 116, "Cambodian Riel", 2)},</v>
+        <v>{ KHR = new Currency("KHR", 116, "Cambodian Riel", 2) },</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -5048,13 +5060,13 @@
       <c r="H79" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="I79" s="3" t="str">
+      <c r="I79" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KMF { get; private set; }</v>
       </c>
-      <c r="J79" s="3" t="str">
+      <c r="J79" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KMF = new Currency("KMF", 174, "Comoro Franc", 0)},</v>
+        <v>{ KMF = new Currency("KMF", 174, "Comoro Franc", 0) },</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -5082,13 +5094,13 @@
       <c r="H80" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="I80" s="3" t="str">
+      <c r="I80" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KPW { get; private set; }</v>
       </c>
-      <c r="J80" s="3" t="str">
+      <c r="J80" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KPW = new Currency("KPW", 408, "North Korean Won", 2)},</v>
+        <v>{ KPW = new Currency("KPW", 408, "North Korean Won", 2) },</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -5116,13 +5128,13 @@
       <c r="H81" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="I81" s="3" t="str">
+      <c r="I81" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KRW { get; private set; }</v>
       </c>
-      <c r="J81" s="3" t="str">
+      <c r="J81" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KRW = new Currency("KRW", 410, "South Korean Won", 0)},</v>
+        <v>{ KRW = new Currency("KRW", 410, "South Korean Won", 0) },</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -5150,13 +5162,13 @@
       <c r="H82" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="I82" s="3" t="str">
+      <c r="I82" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KWD { get; private set; }</v>
       </c>
-      <c r="J82" s="3" t="str">
+      <c r="J82" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KWD = new Currency("KWD", 414, "Kuwaiti Dinar", 3)},</v>
+        <v>{ KWD = new Currency("KWD", 414, "Kuwaiti Dinar", 3) },</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -5184,13 +5196,13 @@
       <c r="H83" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="I83" s="3" t="str">
+      <c r="I83" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KYD { get; private set; }</v>
       </c>
-      <c r="J83" s="3" t="str">
+      <c r="J83" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KYD = new Currency("KYD", 136, "Cayman Islands Dollar", 2)},</v>
+        <v>{ KYD = new Currency("KYD", 136, "Cayman Islands Dollar", 2) },</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -5218,13 +5230,13 @@
       <c r="H84" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="I84" s="3" t="str">
+      <c r="I84" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency KZT { get; private set; }</v>
       </c>
-      <c r="J84" s="3" t="str">
+      <c r="J84" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{KZT = new Currency("KZT", 398, "Kazakhstani Tenge", 2)},</v>
+        <v>{ KZT = new Currency("KZT", 398, "Kazakhstani Tenge", 2) },</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -5252,13 +5264,13 @@
       <c r="H85" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="I85" s="3" t="str">
+      <c r="I85" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency LAK { get; private set; }</v>
       </c>
-      <c r="J85" s="3" t="str">
+      <c r="J85" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{LAK = new Currency("LAK", 418, "Lao Kip", 2)},</v>
+        <v>{ LAK = new Currency("LAK", 418, "Lao Kip", 2) },</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -5286,13 +5298,13 @@
       <c r="H86" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="I86" s="3" t="str">
+      <c r="I86" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency LBP { get; private set; }</v>
       </c>
-      <c r="J86" s="3" t="str">
+      <c r="J86" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{LBP = new Currency("LBP", 422, "Lebanese Pound", 0)},</v>
+        <v>{ LBP = new Currency("LBP", 422, "Lebanese Pound", 0) },</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -5320,13 +5332,13 @@
       <c r="H87" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="I87" s="3" t="str">
+      <c r="I87" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency LKR { get; private set; }</v>
       </c>
-      <c r="J87" s="3" t="str">
+      <c r="J87" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{LKR = new Currency("LKR", 144, "Sri Lanka Rupee", 2)},</v>
+        <v>{ LKR = new Currency("LKR", 144, "Sri Lanka Rupee", 2) },</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -5354,13 +5366,13 @@
       <c r="H88" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="I88" s="3" t="str">
+      <c r="I88" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency LRD { get; private set; }</v>
       </c>
-      <c r="J88" s="3" t="str">
+      <c r="J88" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{LRD = new Currency("LRD", 430, "Liberian Dollar", 2)},</v>
+        <v>{ LRD = new Currency("LRD", 430, "Liberian Dollar", 2) },</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -5388,13 +5400,13 @@
       <c r="H89" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="I89" s="3" t="str">
+      <c r="I89" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency LSL { get; private set; }</v>
       </c>
-      <c r="J89" s="3" t="str">
+      <c r="J89" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{LSL = new Currency("LSL", 426, "Lesotho Loti", 2)},</v>
+        <v>{ LSL = new Currency("LSL", 426, "Lesotho Loti", 2) },</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -5422,13 +5434,13 @@
       <c r="H90" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="I90" s="3" t="str">
+      <c r="I90" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency LTL { get; private set; }</v>
       </c>
-      <c r="J90" s="3" t="str">
+      <c r="J90" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{LTL = new Currency("LTL", 440, "Lithuanian Litas", 2)},</v>
+        <v>{ LTL = new Currency("LTL", 440, "Lithuanian Litas", 2) },</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -5456,13 +5468,13 @@
       <c r="H91" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="I91" s="3" t="str">
+      <c r="I91" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency LVL { get; private set; }</v>
       </c>
-      <c r="J91" s="3" t="str">
+      <c r="J91" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{LVL = new Currency("LVL", 428, "Latvian Lats", 2)},</v>
+        <v>{ LVL = new Currency("LVL", 428, "Latvian Lats", 2) },</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -5490,13 +5502,13 @@
       <c r="H92" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="I92" s="3" t="str">
+      <c r="I92" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency LYD { get; private set; }</v>
       </c>
-      <c r="J92" s="3" t="str">
+      <c r="J92" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{LYD = new Currency("LYD", 434, "Libyan Dinar", 3)},</v>
+        <v>{ LYD = new Currency("LYD", 434, "Libyan Dinar", 3) },</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -5524,13 +5536,13 @@
       <c r="H93" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="I93" s="3" t="str">
+      <c r="I93" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MAD { get; private set; }</v>
       </c>
-      <c r="J93" s="3" t="str">
+      <c r="J93" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MAD = new Currency("MAD", 504, "Moroccan Dirham", 2)},</v>
+        <v>{ MAD = new Currency("MAD", 504, "Moroccan Dirham", 2) },</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -5555,13 +5567,13 @@
       <c r="G94" s="3">
         <v>2</v>
       </c>
-      <c r="I94" s="3" t="str">
+      <c r="I94" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MDL { get; private set; }</v>
       </c>
-      <c r="J94" s="3" t="str">
+      <c r="J94" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MDL = new Currency("MDL", 498, "Moldovan Leu", 2)},</v>
+        <v>{ MDL = new Currency("MDL", 498, "Moldovan Leu", 2) },</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -5586,13 +5598,13 @@
       <c r="G95" s="3">
         <v>0</v>
       </c>
-      <c r="I95" s="3" t="str">
+      <c r="I95" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MGA { get; private set; }</v>
       </c>
-      <c r="J95" s="3" t="str">
+      <c r="J95" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MGA = new Currency("MGA", 969, "Malagasy Ariary", 0)},</v>
+        <v>{ MGA = new Currency("MGA", 969, "Malagasy Ariary", 0) },</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -5617,13 +5629,13 @@
       <c r="G96" s="3">
         <v>2</v>
       </c>
-      <c r="I96" s="3" t="str">
+      <c r="I96" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MKD { get; private set; }</v>
       </c>
-      <c r="J96" s="3" t="str">
+      <c r="J96" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MKD = new Currency("MKD", 807, "Macedonian Denar", 2)},</v>
+        <v>{ MKD = new Currency("MKD", 807, "Macedonian Denar", 2) },</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -5651,13 +5663,13 @@
       <c r="H97" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="I97" s="3" t="str">
+      <c r="I97" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MMK { get; private set; }</v>
       </c>
-      <c r="J97" s="3" t="str">
+      <c r="J97" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MMK = new Currency("MMK", 104, "Myanma Kyat", 2)},</v>
+        <v>{ MMK = new Currency("MMK", 104, "Myanma Kyat", 2) },</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -5685,13 +5697,13 @@
       <c r="H98" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="I98" s="3" t="str">
+      <c r="I98" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MNT { get; private set; }</v>
       </c>
-      <c r="J98" s="3" t="str">
+      <c r="J98" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MNT = new Currency("MNT", 496, "Mongolian Tugrik", 2)},</v>
+        <v>{ MNT = new Currency("MNT", 496, "Mongolian Tugrik", 2) },</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -5719,13 +5731,13 @@
       <c r="H99" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="I99" s="3" t="str">
+      <c r="I99" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MOP { get; private set; }</v>
       </c>
-      <c r="J99" s="3" t="str">
+      <c r="J99" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MOP = new Currency("MOP", 446, "Macanese Pataca", 2)},</v>
+        <v>{ MOP = new Currency("MOP", 446, "Macanese Pataca", 2) },</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -5753,13 +5765,13 @@
       <c r="H100" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="I100" s="3" t="str">
+      <c r="I100" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MRO { get; private set; }</v>
       </c>
-      <c r="J100" s="3" t="str">
+      <c r="J100" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MRO = new Currency("MRO", 478, "Mauritanian Ouguiya", 0)},</v>
+        <v>{ MRO = new Currency("MRO", 478, "Mauritanian Ouguiya", 0) },</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -5787,13 +5799,13 @@
       <c r="H101" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="I101" s="3" t="str">
+      <c r="I101" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MUR { get; private set; }</v>
       </c>
-      <c r="J101" s="3" t="str">
+      <c r="J101" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MUR = new Currency("MUR", 480, "Mauritius Rupee", 0)},</v>
+        <v>{ MUR = new Currency("MUR", 480, "Mauritius Rupee", 0) },</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -5821,13 +5833,13 @@
       <c r="H102" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="I102" s="3" t="str">
+      <c r="I102" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MVR { get; private set; }</v>
       </c>
-      <c r="J102" s="3" t="str">
+      <c r="J102" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MVR = new Currency("MVR", 462, "Maldivian Rufiyaa", 2)},</v>
+        <v>{ MVR = new Currency("MVR", 462, "Maldivian Rufiyaa", 2) },</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -5855,13 +5867,13 @@
       <c r="H103" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="I103" s="3" t="str">
+      <c r="I103" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MWK { get; private set; }</v>
       </c>
-      <c r="J103" s="3" t="str">
+      <c r="J103" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MWK = new Currency("MWK", 454, "Malawian Kwacha", 2)},</v>
+        <v>{ MWK = new Currency("MWK", 454, "Malawian Kwacha", 2) },</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -5889,13 +5901,13 @@
       <c r="H104" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="I104" s="3" t="str">
+      <c r="I104" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MXN { get; private set; }</v>
       </c>
-      <c r="J104" s="3" t="str">
+      <c r="J104" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MXN = new Currency("MXN", 484, "Mexican Peso", 2)},</v>
+        <v>{ MXN = new Currency("MXN", 484, "Mexican Peso", 2) },</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -5914,13 +5926,13 @@
       <c r="G105" s="3">
         <v>2</v>
       </c>
-      <c r="I105" s="3" t="str">
+      <c r="I105" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MXV { get; private set; }</v>
       </c>
-      <c r="J105" s="3" t="str">
+      <c r="J105" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MXV = new Currency("MXV", 979, "Mexican Unidad de Inversion (UDI)", 2)},</v>
+        <v>{ MXV = new Currency("MXV", 979, "Mexican Unidad de Inversion (UDI)", 2) },</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -5948,13 +5960,13 @@
       <c r="H106" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="I106" s="3" t="str">
+      <c r="I106" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MYR { get; private set; }</v>
       </c>
-      <c r="J106" s="3" t="str">
+      <c r="J106" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MYR = new Currency("MYR", 458, "Malaysian Ringgit", 2)},</v>
+        <v>{ MYR = new Currency("MYR", 458, "Malaysian Ringgit", 2) },</v>
       </c>
     </row>
     <row r="107" spans="1:10">
@@ -5982,13 +5994,13 @@
       <c r="H107" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="I107" s="3" t="str">
+      <c r="I107" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency MZN { get; private set; }</v>
       </c>
-      <c r="J107" s="3" t="str">
+      <c r="J107" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{MZN = new Currency("MZN", 943, "Mozambican Metical", 2)},</v>
+        <v>{ MZN = new Currency("MZN", 943, "Mozambican Metical", 2) },</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -6016,13 +6028,13 @@
       <c r="H108" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="I108" s="3" t="str">
+      <c r="I108" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency NAD { get; private set; }</v>
       </c>
-      <c r="J108" s="3" t="str">
+      <c r="J108" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{NAD = new Currency("NAD", 516, "Namibia Dollar", 2)},</v>
+        <v>{ NAD = new Currency("NAD", 516, "Namibia Dollar", 2) },</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -6050,13 +6062,13 @@
       <c r="H109" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="I109" s="3" t="str">
+      <c r="I109" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency NGN { get; private set; }</v>
       </c>
-      <c r="J109" s="3" t="str">
+      <c r="J109" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{NGN = new Currency("NGN", 566, "Nigerian Naira", 2)},</v>
+        <v>{ NGN = new Currency("NGN", 566, "Nigerian Naira", 2) },</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -6084,13 +6096,13 @@
       <c r="H110" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="I110" s="3" t="str">
+      <c r="I110" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency NIO { get; private set; }</v>
       </c>
-      <c r="J110" s="3" t="str">
+      <c r="J110" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{NIO = new Currency("NIO", 558, "Nicaraguan Córdoba", 2)},</v>
+        <v>{ NIO = new Currency("NIO", 558, "Nicaraguan Córdoba", 2) },</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -6118,13 +6130,13 @@
       <c r="H111" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="I111" s="3" t="str">
+      <c r="I111" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency NOK { get; private set; }</v>
       </c>
-      <c r="J111" s="3" t="str">
+      <c r="J111" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{NOK = new Currency("NOK", 578, "Norwegian Krone", 2)},</v>
+        <v>{ NOK = new Currency("NOK", 578, "Norwegian Krone", 2) },</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -6152,13 +6164,13 @@
       <c r="H112" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="I112" s="3" t="str">
+      <c r="I112" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency NPR { get; private set; }</v>
       </c>
-      <c r="J112" s="3" t="str">
+      <c r="J112" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{NPR = new Currency("NPR", 524, "Nepalese Rupee", 2)},</v>
+        <v>{ NPR = new Currency("NPR", 524, "Nepalese Rupee", 2) },</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -6186,13 +6198,13 @@
       <c r="H113" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="I113" s="3" t="str">
+      <c r="I113" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency NZD { get; private set; }</v>
       </c>
-      <c r="J113" s="3" t="str">
+      <c r="J113" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{NZD = new Currency("NZD", 554, "New Zealand Dollar", 2)},</v>
+        <v>{ NZD = new Currency("NZD", 554, "New Zealand Dollar", 2) },</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -6220,13 +6232,13 @@
       <c r="H114" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="I114" s="3" t="str">
+      <c r="I114" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency OMR { get; private set; }</v>
       </c>
-      <c r="J114" s="3" t="str">
+      <c r="J114" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{OMR = new Currency("OMR", 512, "Omani Rial", 3)},</v>
+        <v>{ OMR = new Currency("OMR", 512, "Omani Rial", 3) },</v>
       </c>
     </row>
     <row r="115" spans="1:10">
@@ -6254,13 +6266,13 @@
       <c r="H115" s="6" t="s">
         <v>650</v>
       </c>
-      <c r="I115" s="3" t="str">
+      <c r="I115" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency PAB { get; private set; }</v>
       </c>
-      <c r="J115" s="3" t="str">
+      <c r="J115" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{PAB = new Currency("PAB", 590, "Panamanian Balboa", 2)},</v>
+        <v>{ PAB = new Currency("PAB", 590, "Panamanian Balboa", 2) },</v>
       </c>
     </row>
     <row r="116" spans="1:10">
@@ -6288,13 +6300,13 @@
       <c r="H116" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="I116" s="3" t="str">
+      <c r="I116" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency PEN { get; private set; }</v>
       </c>
-      <c r="J116" s="3" t="str">
+      <c r="J116" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{PEN = new Currency("PEN", 604, "Peruvian Nuevo Sol", 2)},</v>
+        <v>{ PEN = new Currency("PEN", 604, "Peruvian Nuevo Sol", 2) },</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -6322,13 +6334,13 @@
       <c r="H117" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="I117" s="3" t="str">
+      <c r="I117" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency PGK { get; private set; }</v>
       </c>
-      <c r="J117" s="3" t="str">
+      <c r="J117" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{PGK = new Currency("PGK", 598, "Papua New Guinean Kina", 2)},</v>
+        <v>{ PGK = new Currency("PGK", 598, "Papua New Guinean Kina", 2) },</v>
       </c>
     </row>
     <row r="118" spans="1:10">
@@ -6356,13 +6368,13 @@
       <c r="H118" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="I118" s="3" t="str">
+      <c r="I118" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency PHP { get; private set; }</v>
       </c>
-      <c r="J118" s="3" t="str">
+      <c r="J118" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{PHP = new Currency("PHP", 608, "Philippine Peso", 2)},</v>
+        <v>{ PHP = new Currency("PHP", 608, "Philippine Peso", 2) },</v>
       </c>
     </row>
     <row r="119" spans="1:10">
@@ -6390,13 +6402,13 @@
       <c r="H119" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="I119" s="3" t="str">
+      <c r="I119" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency PKR { get; private set; }</v>
       </c>
-      <c r="J119" s="3" t="str">
+      <c r="J119" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{PKR = new Currency("PKR", 586, "Pakistani Rupee", 2)},</v>
+        <v>{ PKR = new Currency("PKR", 586, "Pakistani Rupee", 2) },</v>
       </c>
     </row>
     <row r="120" spans="1:10">
@@ -6424,13 +6436,13 @@
       <c r="H120" s="3" t="s">
         <v>652</v>
       </c>
-      <c r="I120" s="3" t="str">
+      <c r="I120" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency PLN { get; private set; }</v>
       </c>
-      <c r="J120" s="3" t="str">
+      <c r="J120" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{PLN = new Currency("PLN", 985, "Polish Złoty", 2)},</v>
+        <v>{ PLN = new Currency("PLN", 985, "Polish Złoty", 2) },</v>
       </c>
     </row>
     <row r="121" spans="1:10">
@@ -6458,13 +6470,13 @@
       <c r="H121" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="I121" s="3" t="str">
+      <c r="I121" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency PYG { get; private set; }</v>
       </c>
-      <c r="J121" s="3" t="str">
+      <c r="J121" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{PYG = new Currency("PYG", 600, "Paraguayan Guaraní", 2)},</v>
+        <v>{ PYG = new Currency("PYG", 600, "Paraguayan Guaraní", 2) },</v>
       </c>
     </row>
     <row r="122" spans="1:10">
@@ -6492,13 +6504,13 @@
       <c r="H122" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="I122" s="3" t="str">
+      <c r="I122" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency QAR { get; private set; }</v>
       </c>
-      <c r="J122" s="3" t="str">
+      <c r="J122" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{QAR = new Currency("QAR", 634, "Qatari Riyal", 2)},</v>
+        <v>{ QAR = new Currency("QAR", 634, "Qatari Riyal", 2) },</v>
       </c>
     </row>
     <row r="123" spans="1:10">
@@ -6526,13 +6538,13 @@
       <c r="H123" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="I123" s="3" t="str">
+      <c r="I123" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency RON { get; private set; }</v>
       </c>
-      <c r="J123" s="3" t="str">
+      <c r="J123" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{RON = new Currency("RON", 946, "Romanian Leu", 2)},</v>
+        <v>{ RON = new Currency("RON", 946, "Romanian Leu", 2) },</v>
       </c>
     </row>
     <row r="124" spans="1:10">
@@ -6560,13 +6572,13 @@
       <c r="H124" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="I124" s="3" t="str">
+      <c r="I124" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency RSD { get; private set; }</v>
       </c>
-      <c r="J124" s="3" t="str">
+      <c r="J124" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{RSD = new Currency("RSD", 941, "Serbian Dinar", 2)},</v>
+        <v>{ RSD = new Currency("RSD", 941, "Serbian Dinar", 2) },</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -6594,13 +6606,13 @@
       <c r="H125" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="I125" s="3" t="str">
+      <c r="I125" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency RUB { get; private set; }</v>
       </c>
-      <c r="J125" s="3" t="str">
+      <c r="J125" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{RUB = new Currency("RUB", 643, "Russian Ruble", 2)},</v>
+        <v>{ RUB = new Currency("RUB", 643, "Russian Ruble", 2) },</v>
       </c>
     </row>
     <row r="126" spans="1:10">
@@ -6628,13 +6640,13 @@
       <c r="H126" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="I126" s="3" t="str">
+      <c r="I126" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency RWF { get; private set; }</v>
       </c>
-      <c r="J126" s="3" t="str">
+      <c r="J126" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{RWF = new Currency("RWF", 646, "Rwanda Franc", 0)},</v>
+        <v>{ RWF = new Currency("RWF", 646, "Rwanda Franc", 0) },</v>
       </c>
     </row>
     <row r="127" spans="1:10">
@@ -6662,13 +6674,13 @@
       <c r="H127" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="I127" s="3" t="str">
+      <c r="I127" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency SAR { get; private set; }</v>
       </c>
-      <c r="J127" s="3" t="str">
+      <c r="J127" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{SAR = new Currency("SAR", 682, "Saudi Riyal", 2)},</v>
+        <v>{ SAR = new Currency("SAR", 682, "Saudi Riyal", 2) },</v>
       </c>
     </row>
     <row r="128" spans="1:10">
@@ -6696,13 +6708,13 @@
       <c r="H128" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="I128" s="3" t="str">
+      <c r="I128" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency SBD { get; private set; }</v>
       </c>
-      <c r="J128" s="3" t="str">
+      <c r="J128" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{SBD = new Currency("SBD", 90, "Solomon Islands Dollar", 2)},</v>
+        <v>{ SBD = new Currency("SBD", 90, "Solomon Islands Dollar", 2) },</v>
       </c>
     </row>
     <row r="129" spans="1:10">
@@ -6730,13 +6742,13 @@
       <c r="H129" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="I129" s="3" t="str">
+      <c r="I129" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency SCR { get; private set; }</v>
       </c>
-      <c r="J129" s="3" t="str">
+      <c r="J129" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{SCR = new Currency("SCR", 690, "Seychelles Rupee", 2)},</v>
+        <v>{ SCR = new Currency("SCR", 690, "Seychelles Rupee", 2) },</v>
       </c>
     </row>
     <row r="130" spans="1:10">
@@ -6761,13 +6773,13 @@
       <c r="G130" s="3">
         <v>2</v>
       </c>
-      <c r="I130" s="3" t="str">
+      <c r="I130" s="8" t="str">
         <f t="shared" si="2"/>
         <v>public static Currency SDG { get; private set; }</v>
       </c>
-      <c r="J130" s="3" t="str">
+      <c r="J130" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>{SDG = new Currency("SDG", 938, "Sudanese Pound", 2)},</v>
+        <v>{ SDG = new Currency("SDG", 938, "Sudanese Pound", 2) },</v>
       </c>
     </row>
     <row r="131" spans="1:10">
@@ -6795,13 +6807,13 @@
       <c r="H131" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="I131" s="3" t="str">
-        <f t="shared" ref="I131:I181" si="4">CONCATENATE("public static Currency ", A131, " { get; private set; }")</f>
+      <c r="I131" s="8" t="str">
+        <f t="shared" ref="I131:I182" si="4">CONCATENATE("public static Currency ", A131, " { get; private set; }")</f>
         <v>public static Currency SEK { get; private set; }</v>
       </c>
-      <c r="J131" s="3" t="str">
-        <f t="shared" ref="J131:J181" si="5">CONCATENATE("{", A131, " = new Currency(""",A131,""", ", B131,", """, C131,""", ",G131, ")},")</f>
-        <v>{SEK = new Currency("SEK", 752, "Swedish Krona", 2)},</v>
+      <c r="J131" s="8" t="str">
+        <f t="shared" ref="J131:J182" si="5">CONCATENATE("{ ", A131, " = new Currency(""",A131,""", ", B131,", """, C131,""", ",G131, ") },")</f>
+        <v>{ SEK = new Currency("SEK", 752, "Swedish Krona", 2) },</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -6829,13 +6841,13 @@
       <c r="H132" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="I132" s="3" t="str">
+      <c r="I132" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency SGD { get; private set; }</v>
       </c>
-      <c r="J132" s="3" t="str">
+      <c r="J132" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{SGD = new Currency("SGD", 702, "Singapore Dollar", 2)},</v>
+        <v>{ SGD = new Currency("SGD", 702, "Singapore Dollar", 2) },</v>
       </c>
     </row>
     <row r="133" spans="1:10">
@@ -6863,13 +6875,13 @@
       <c r="H133" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="I133" s="3" t="str">
+      <c r="I133" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency SHP { get; private set; }</v>
       </c>
-      <c r="J133" s="3" t="str">
+      <c r="J133" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{SHP = new Currency("SHP", 654, "Saint Helena Pound", 2)},</v>
+        <v>{ SHP = new Currency("SHP", 654, "Saint Helena Pound", 2) },</v>
       </c>
     </row>
     <row r="134" spans="1:10">
@@ -6897,13 +6909,13 @@
       <c r="H134" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="I134" s="3" t="str">
+      <c r="I134" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency SLL { get; private set; }</v>
       </c>
-      <c r="J134" s="3" t="str">
+      <c r="J134" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{SLL = new Currency("SLL", 694, "Sierra Leonean Leone", 2)},</v>
+        <v>{ SLL = new Currency("SLL", 694, "Sierra Leonean Leone", 2) },</v>
       </c>
     </row>
     <row r="135" spans="1:10">
@@ -6931,13 +6943,13 @@
       <c r="H135" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="I135" s="3" t="str">
+      <c r="I135" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency SOS { get; private set; }</v>
       </c>
-      <c r="J135" s="3" t="str">
+      <c r="J135" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{SOS = new Currency("SOS", 706, "Somali Shilling", 2)},</v>
+        <v>{ SOS = new Currency("SOS", 706, "Somali Shilling", 2) },</v>
       </c>
     </row>
     <row r="136" spans="1:10">
@@ -6962,1408 +6974,1439 @@
       <c r="G136" s="3">
         <v>2</v>
       </c>
-      <c r="I136" s="3" t="str">
+      <c r="I136" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency SRD { get; private set; }</v>
       </c>
-      <c r="J136" s="3" t="str">
+      <c r="J136" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{SRD = new Currency("SRD", 968, "Surinamese Dollar", 2)},</v>
+        <v>{ SRD = new Currency("SRD", 968, "Surinamese Dollar", 2) },</v>
       </c>
     </row>
     <row r="137" spans="1:10">
       <c r="A137" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="B137" s="2">
+        <v>728</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="F137" s="3">
+        <v>100</v>
+      </c>
+      <c r="G137" s="3">
+        <v>2</v>
+      </c>
+      <c r="I137" s="8" t="str">
+        <f t="shared" ref="I137" si="6">CONCATENATE("public static Currency ", A137, " { get; private set; }")</f>
+        <v>public static Currency SSP { get; private set; }</v>
+      </c>
+      <c r="J137" s="8" t="str">
+        <f t="shared" ref="J137" si="7">CONCATENATE("{ ", A137, " = new Currency(""",A137,""", ", B137,", """, C137,""", ",G137, ") },")</f>
+        <v>{ SSP = new Currency("SSP", 728, "South Sudanese Pound", 2) },</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
+      <c r="A138" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B137" s="2">
+      <c r="B138" s="2">
         <v>678</v>
       </c>
-      <c r="C137" s="3" t="s">
+      <c r="C138" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="D138" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="E137" s="3" t="s">
+      <c r="E138" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="F137" s="3">
-        <v>100</v>
-      </c>
-      <c r="G137" s="3">
-        <v>2</v>
-      </c>
-      <c r="H137" s="3" t="s">
+      <c r="F138" s="3">
+        <v>100</v>
+      </c>
+      <c r="G138" s="3">
+        <v>2</v>
+      </c>
+      <c r="H138" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="I137" s="3" t="str">
+      <c r="I138" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency STD { get; private set; }</v>
       </c>
-      <c r="J137" s="3" t="str">
+      <c r="J138" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{STD = new Currency("STD", 678, "São Tomé And Príncipe Dobra", 2)},</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10">
-      <c r="A138" s="2" t="s">
+        <v>{ STD = new Currency("STD", 678, "São Tomé And Príncipe Dobra", 2) },</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
+      <c r="A139" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B138" s="2">
+      <c r="B139" s="2">
         <v>222</v>
       </c>
-      <c r="C138" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="D138" s="3" t="s">
+      <c r="D139" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="E138" s="3" t="s">
+      <c r="E139" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="F138" s="3">
-        <v>100</v>
-      </c>
-      <c r="G138" s="3">
-        <v>2</v>
-      </c>
-      <c r="H138" s="3" t="s">
+      <c r="F139" s="3">
+        <v>100</v>
+      </c>
+      <c r="G139" s="3">
+        <v>2</v>
+      </c>
+      <c r="H139" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="I138" s="3" t="str">
+      <c r="I139" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency SVC { get; private set; }</v>
       </c>
-      <c r="J138" s="3" t="str">
+      <c r="J139" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{SVC = new Currency("SVC", 222, "Salvadoran Colón", 2)},</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10">
-      <c r="A139" s="2" t="s">
+        <v>{ SVC = new Currency("SVC", 222, "Salvadoran Colón", 2) },</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
+      <c r="A140" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B140" s="2">
         <v>760</v>
       </c>
-      <c r="C139" s="3" t="s">
+      <c r="C140" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D139" s="3" t="s">
+      <c r="D140" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="E139" s="3" t="s">
+      <c r="E140" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="F139" s="3">
-        <v>100</v>
-      </c>
-      <c r="G139" s="3">
-        <v>2</v>
-      </c>
-      <c r="I139" s="3" t="str">
+      <c r="F140" s="3">
+        <v>100</v>
+      </c>
+      <c r="G140" s="3">
+        <v>2</v>
+      </c>
+      <c r="I140" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency SYP { get; private set; }</v>
       </c>
-      <c r="J139" s="3" t="str">
+      <c r="J140" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{SYP = new Currency("SYP", 760, "Syrian Pound", 2)},</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10">
-      <c r="A140" s="2" t="s">
+        <v>{ SYP = new Currency("SYP", 760, "Syrian Pound", 2) },</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
+      <c r="A141" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B140" s="2">
+      <c r="B141" s="2">
         <v>748</v>
       </c>
-      <c r="C140" s="3" t="s">
+      <c r="C141" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="D140" s="3" t="s">
+      <c r="D141" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E140" s="3" t="s">
+      <c r="E141" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F140" s="3">
-        <v>100</v>
-      </c>
-      <c r="G140" s="3">
-        <v>2</v>
-      </c>
-      <c r="H140" s="1" t="s">
+      <c r="F141" s="3">
+        <v>100</v>
+      </c>
+      <c r="G141" s="3">
+        <v>2</v>
+      </c>
+      <c r="H141" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="I140" s="3" t="str">
+      <c r="I141" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency SZL { get; private set; }</v>
       </c>
-      <c r="J140" s="3" t="str">
+      <c r="J141" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{SZL = new Currency("SZL", 748, "Swazi Lilangeni", 2)},</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10">
-      <c r="A141" s="2" t="s">
+        <v>{ SZL = new Currency("SZL", 748, "Swazi Lilangeni", 2) },</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
+      <c r="A142" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B141" s="2">
+      <c r="B142" s="2">
         <v>764</v>
       </c>
-      <c r="C141" s="3" t="s">
+      <c r="C142" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="D141" s="3" t="s">
+      <c r="D142" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="E141" s="3" t="s">
+      <c r="E142" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="F141" s="3">
-        <v>100</v>
-      </c>
-      <c r="G141" s="3">
-        <v>2</v>
-      </c>
-      <c r="H141" s="3" t="s">
+      <c r="F142" s="3">
+        <v>100</v>
+      </c>
+      <c r="G142" s="3">
+        <v>2</v>
+      </c>
+      <c r="H142" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="I141" s="3" t="str">
+      <c r="I142" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency THB { get; private set; }</v>
       </c>
-      <c r="J141" s="3" t="str">
+      <c r="J142" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{THB = new Currency("THB", 764, "Thai Baht", 2)},</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10">
-      <c r="A142" s="2" t="s">
+        <v>{ THB = new Currency("THB", 764, "Thai Baht", 2) },</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
+      <c r="A143" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B142" s="2">
+      <c r="B143" s="2">
         <v>972</v>
       </c>
-      <c r="C142" s="3" t="s">
+      <c r="C143" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="D142" s="3" t="s">
+      <c r="D143" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E142" s="3" t="s">
+      <c r="E143" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="F142" s="3">
-        <v>100</v>
-      </c>
-      <c r="G142" s="3">
-        <v>2</v>
-      </c>
-      <c r="I142" s="3" t="str">
+      <c r="F143" s="3">
+        <v>100</v>
+      </c>
+      <c r="G143" s="3">
+        <v>2</v>
+      </c>
+      <c r="I143" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency TJS { get; private set; }</v>
       </c>
-      <c r="J142" s="3" t="str">
+      <c r="J143" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{TJS = new Currency("TJS", 972, "Tajikistani Somoni", 2)},</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10">
-      <c r="A143" s="2" t="s">
+        <v>{ TJS = new Currency("TJS", 972, "Tajikistani Somoni", 2) },</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
+      <c r="A144" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B143" s="2">
+      <c r="B144" s="2">
         <v>934</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="D143" s="3" t="s">
+      <c r="D144" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="E143" s="3" t="s">
+      <c r="E144" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="F143" s="3">
-        <v>100</v>
-      </c>
-      <c r="G143" s="3">
-        <v>2</v>
-      </c>
-      <c r="H143" s="3" t="s">
+      <c r="F144" s="3">
+        <v>100</v>
+      </c>
+      <c r="G144" s="3">
+        <v>2</v>
+      </c>
+      <c r="H144" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="I143" s="3" t="str">
+      <c r="I144" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency TMT { get; private set; }</v>
       </c>
-      <c r="J143" s="3" t="str">
+      <c r="J144" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{TMT = new Currency("TMT", 934, "Turkmenistani Manat", 2)},</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10">
-      <c r="A144" s="2" t="s">
+        <v>{ TMT = new Currency("TMT", 934, "Turkmenistani Manat", 2) },</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
+      <c r="A145" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B144" s="2">
+      <c r="B145" s="2">
         <v>788</v>
       </c>
-      <c r="C144" s="3" t="s">
+      <c r="C145" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D145" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="E144" s="3" t="s">
+      <c r="E145" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="F144" s="4">
+      <c r="F145" s="4">
         <v>1000</v>
       </c>
-      <c r="G144" s="3">
+      <c r="G145" s="3">
         <v>3</v>
       </c>
-      <c r="H144" s="3" t="s">
+      <c r="H145" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="I144" s="3" t="str">
+      <c r="I145" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency TND { get; private set; }</v>
       </c>
-      <c r="J144" s="3" t="str">
+      <c r="J145" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{TND = new Currency("TND", 788, "Tunisian Dinar", 3)},</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10">
-      <c r="A145" s="2" t="s">
+        <v>{ TND = new Currency("TND", 788, "Tunisian Dinar", 3) },</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="A146" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B146" s="2">
         <v>776</v>
       </c>
-      <c r="C145" s="3" t="s">
+      <c r="C146" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="D145" s="3" t="s">
+      <c r="D146" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="E145" s="3" t="s">
+      <c r="E146" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="F145" s="3">
-        <v>100</v>
-      </c>
-      <c r="G145" s="3">
-        <v>2</v>
-      </c>
-      <c r="H145" s="3" t="s">
+      <c r="F146" s="3">
+        <v>100</v>
+      </c>
+      <c r="G146" s="3">
+        <v>2</v>
+      </c>
+      <c r="H146" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="I145" s="3" t="str">
+      <c r="I146" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency TOP { get; private set; }</v>
       </c>
-      <c r="J145" s="3" t="str">
+      <c r="J146" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{TOP = new Currency("TOP", 776, "Tongan Paʻanga", 2)},</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10">
-      <c r="A146" s="2" t="s">
+        <v>{ TOP = new Currency("TOP", 776, "Tongan Paʻanga", 2) },</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
+      <c r="A147" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B147" s="2">
         <v>949</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="C147" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D146" s="3" t="s">
+      <c r="D147" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="E146" s="3" t="s">
+      <c r="E147" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="F146" s="3">
-        <v>100</v>
-      </c>
-      <c r="G146" s="3">
-        <v>2</v>
-      </c>
-      <c r="H146" s="3" t="s">
+      <c r="F147" s="3">
+        <v>100</v>
+      </c>
+      <c r="G147" s="3">
+        <v>2</v>
+      </c>
+      <c r="H147" s="3" t="s">
         <v>659</v>
       </c>
-      <c r="I146" s="3" t="str">
+      <c r="I147" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency TRY { get; private set; }</v>
       </c>
-      <c r="J146" s="3" t="str">
+      <c r="J147" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{TRY = new Currency("TRY", 949, "Turkish Lira", 2)},</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10">
-      <c r="A147" s="2" t="s">
+        <v>{ TRY = new Currency("TRY", 949, "Turkish Lira", 2) },</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
+      <c r="A148" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B148" s="2">
         <v>780</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D148" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="E147" s="3" t="s">
+      <c r="E148" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F147" s="3">
-        <v>100</v>
-      </c>
-      <c r="G147" s="3">
-        <v>2</v>
-      </c>
-      <c r="H147" s="3" t="s">
+      <c r="F148" s="3">
+        <v>100</v>
+      </c>
+      <c r="G148" s="3">
+        <v>2</v>
+      </c>
+      <c r="H148" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="I147" s="3" t="str">
+      <c r="I148" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency TTD { get; private set; }</v>
       </c>
-      <c r="J147" s="3" t="str">
+      <c r="J148" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{TTD = new Currency("TTD", 780, "Trinidad and Tobago Dollar", 2)},</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10">
-      <c r="A148" s="2" t="s">
+        <v>{ TTD = new Currency("TTD", 780, "Trinidad and Tobago Dollar", 2) },</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
+      <c r="A149" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B149" s="2">
         <v>901</v>
       </c>
-      <c r="C148" s="3" t="s">
+      <c r="C149" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D148" s="3" t="s">
+      <c r="D149" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="E148" s="3" t="s">
+      <c r="E149" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F148" s="3">
-        <v>100</v>
-      </c>
-      <c r="G148" s="3">
-        <v>2</v>
-      </c>
-      <c r="H148" s="3" t="s">
+      <c r="F149" s="3">
+        <v>100</v>
+      </c>
+      <c r="G149" s="3">
+        <v>2</v>
+      </c>
+      <c r="H149" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="I148" s="3" t="str">
+      <c r="I149" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency TWD { get; private set; }</v>
       </c>
-      <c r="J148" s="3" t="str">
+      <c r="J149" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{TWD = new Currency("TWD", 901, "New Taiwan Dollar", 2)},</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10">
-      <c r="A149" s="2" t="s">
+        <v>{ TWD = new Currency("TWD", 901, "New Taiwan Dollar", 2) },</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
+      <c r="A150" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B150" s="2">
         <v>834</v>
       </c>
-      <c r="C149" s="3" t="s">
+      <c r="C150" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D150" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="E149" s="3" t="s">
+      <c r="E150" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="F149" s="3">
-        <v>100</v>
-      </c>
-      <c r="G149" s="3">
-        <v>2</v>
-      </c>
-      <c r="H149" s="3" t="s">
+      <c r="F150" s="3">
+        <v>100</v>
+      </c>
+      <c r="G150" s="3">
+        <v>2</v>
+      </c>
+      <c r="H150" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="I149" s="3" t="str">
+      <c r="I150" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency TZS { get; private set; }</v>
       </c>
-      <c r="J149" s="3" t="str">
+      <c r="J150" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{TZS = new Currency("TZS", 834, "Tanzanian Shilling", 2)},</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10">
-      <c r="A150" s="2" t="s">
+        <v>{ TZS = new Currency("TZS", 834, "Tanzanian Shilling", 2) },</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
+      <c r="A151" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B151" s="2">
         <v>980</v>
       </c>
-      <c r="C150" s="3" t="s">
+      <c r="C151" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="D151" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E150" s="3" t="s">
+      <c r="E151" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="F150" s="3">
-        <v>100</v>
-      </c>
-      <c r="G150" s="3">
-        <v>2</v>
-      </c>
-      <c r="I150" s="3" t="str">
+      <c r="F151" s="3">
+        <v>100</v>
+      </c>
+      <c r="G151" s="3">
+        <v>2</v>
+      </c>
+      <c r="I151" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency UAH { get; private set; }</v>
       </c>
-      <c r="J150" s="3" t="str">
+      <c r="J151" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{UAH = new Currency("UAH", 980, "Ukrainian Hryvnia", 2)},</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10">
-      <c r="A151" s="2" t="s">
+        <v>{ UAH = new Currency("UAH", 980, "Ukrainian Hryvnia", 2) },</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
+      <c r="A152" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B152" s="2">
         <v>800</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="D152" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="E151" s="3" t="s">
+      <c r="E152" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F151" s="3">
-        <v>100</v>
-      </c>
-      <c r="G151" s="3">
+      <c r="F152" s="3">
+        <v>100</v>
+      </c>
+      <c r="G152" s="3">
         <v>0</v>
       </c>
-      <c r="H151" s="3" t="s">
+      <c r="H152" s="3" t="s">
         <v>660</v>
       </c>
-      <c r="I151" s="3" t="str">
+      <c r="I152" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency UGX { get; private set; }</v>
       </c>
-      <c r="J151" s="3" t="str">
+      <c r="J152" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{UGX = new Currency("UGX", 800, "Uganda Shilling", 0)},</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10">
-      <c r="A152" s="2" t="s">
+        <v>{ UGX = new Currency("UGX", 800, "Uganda Shilling", 0) },</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
+      <c r="A153" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B152" s="2">
+      <c r="B153" s="2">
         <v>840</v>
       </c>
-      <c r="C152" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D152" s="3" t="s">
+      <c r="D153" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="E152" s="3" t="s">
+      <c r="E153" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F152" s="3">
-        <v>100</v>
-      </c>
-      <c r="G152" s="3">
-        <v>2</v>
-      </c>
-      <c r="H152" s="3" t="s">
+      <c r="F153" s="3">
+        <v>100</v>
+      </c>
+      <c r="G153" s="3">
+        <v>2</v>
+      </c>
+      <c r="H153" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="I152" s="3" t="str">
+      <c r="I153" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency USD { get; private set; }</v>
       </c>
-      <c r="J152" s="3" t="str">
+      <c r="J153" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{USD = new Currency("USD", 840, "US Dollar", 2)},</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10">
-      <c r="A153" s="2" t="s">
+        <v>{ USD = new Currency("USD", 840, "US Dollar", 2) },</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
+      <c r="A154" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B153" s="2">
+      <c r="B154" s="2">
         <v>997</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="C154" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D153" s="3" t="s">
+      <c r="D154" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="E153" s="3" t="s">
+      <c r="E154" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F153" s="3">
-        <v>100</v>
-      </c>
-      <c r="G153" s="3">
-        <v>2</v>
-      </c>
-      <c r="I153" s="3" t="str">
+      <c r="F154" s="3">
+        <v>100</v>
+      </c>
+      <c r="G154" s="3">
+        <v>2</v>
+      </c>
+      <c r="I154" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency USN { get; private set; }</v>
       </c>
-      <c r="J153" s="3" t="str">
+      <c r="J154" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{USN = new Currency("USN", 997, "US Dollar (Next day)", 2)},</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10">
-      <c r="A154" s="2" t="s">
+        <v>{ USN = new Currency("USN", 997, "US Dollar (Next day)", 2) },</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
+      <c r="A155" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B154" s="2">
+      <c r="B155" s="2">
         <v>998</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D155" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="E154" s="3" t="s">
+      <c r="E155" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F154" s="3">
-        <v>100</v>
-      </c>
-      <c r="G154" s="3">
-        <v>2</v>
-      </c>
-      <c r="I154" s="3" t="str">
+      <c r="F155" s="3">
+        <v>100</v>
+      </c>
+      <c r="G155" s="3">
+        <v>2</v>
+      </c>
+      <c r="I155" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency USS { get; private set; }</v>
       </c>
-      <c r="J154" s="3" t="str">
+      <c r="J155" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{USS = new Currency("USS", 998, "US Dollar (Same day)", 2)},</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10">
-      <c r="A155" s="2" t="s">
+        <v>{ USS = new Currency("USS", 998, "US Dollar (Same day)", 2) },</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
+      <c r="A156" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B155" s="2">
+      <c r="B156" s="2">
         <v>940</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="C156" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D156" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="E155" s="3" t="s">
+      <c r="E156" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F155" s="3">
-        <v>100</v>
-      </c>
-      <c r="G155" s="3">
-        <v>2</v>
-      </c>
-      <c r="I155" s="3" t="str">
+      <c r="F156" s="3">
+        <v>100</v>
+      </c>
+      <c r="G156" s="3">
+        <v>2</v>
+      </c>
+      <c r="I156" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency UYI { get; private set; }</v>
       </c>
-      <c r="J155" s="3" t="str">
+      <c r="J156" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{UYI = new Currency("UYI", 940, "Uruguay Peso en Unidades Indexadas", 2)},</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10">
-      <c r="A156" s="2" t="s">
+        <v>{ UYI = new Currency("UYI", 940, "Uruguay Peso en Unidades Indexadas", 2) },</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10">
+      <c r="A157" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B156" s="2">
+      <c r="B157" s="2">
         <v>858</v>
       </c>
-      <c r="C156" s="3" t="s">
+      <c r="C157" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D157" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E156" s="3" t="s">
+      <c r="E157" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F156" s="3">
-        <v>100</v>
-      </c>
-      <c r="G156" s="3">
-        <v>2</v>
-      </c>
-      <c r="H156" s="3" t="s">
+      <c r="F157" s="3">
+        <v>100</v>
+      </c>
+      <c r="G157" s="3">
+        <v>2</v>
+      </c>
+      <c r="H157" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="I156" s="3" t="str">
+      <c r="I157" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency UYU { get; private set; }</v>
       </c>
-      <c r="J156" s="3" t="str">
+      <c r="J157" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{UYU = new Currency("UYU", 858, "Uruguayan Peso", 2)},</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10">
-      <c r="A157" s="2" t="s">
+        <v>{ UYU = new Currency("UYU", 858, "Uruguayan Peso", 2) },</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10">
+      <c r="A158" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B157" s="2">
+      <c r="B158" s="2">
         <v>860</v>
       </c>
-      <c r="C157" s="3" t="s">
+      <c r="C158" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D158" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E157" s="3" t="s">
+      <c r="E158" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="F157" s="3">
-        <v>100</v>
-      </c>
-      <c r="G157" s="3">
-        <v>2</v>
-      </c>
-      <c r="I157" s="3" t="str">
+      <c r="F158" s="3">
+        <v>100</v>
+      </c>
+      <c r="G158" s="3">
+        <v>2</v>
+      </c>
+      <c r="I158" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency UZS { get; private set; }</v>
       </c>
-      <c r="J157" s="3" t="str">
+      <c r="J158" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{UZS = new Currency("UZS", 860, "Uzbekistani Som", 2)},</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10">
-      <c r="A158" s="2" t="s">
+        <v>{ UZS = new Currency("UZS", 860, "Uzbekistani Som", 2) },</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
+      <c r="A159" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B158" s="2">
+      <c r="B159" s="2">
         <v>937</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="C159" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="D158" s="2" t="s">
+      <c r="D159" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E159" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="F158" s="3">
-        <v>100</v>
-      </c>
-      <c r="G158" s="3">
-        <v>2</v>
-      </c>
-      <c r="H158" s="3" t="s">
+      <c r="F159" s="3">
+        <v>100</v>
+      </c>
+      <c r="G159" s="3">
+        <v>2</v>
+      </c>
+      <c r="H159" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="I158" s="3" t="str">
+      <c r="I159" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency VEF { get; private set; }</v>
       </c>
-      <c r="J158" s="3" t="str">
+      <c r="J159" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{VEF = new Currency("VEF", 937, "Venezuelan Bolívar", 2)},</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10">
-      <c r="A159" s="2" t="s">
+        <v>{ VEF = new Currency("VEF", 937, "Venezuelan Bolívar", 2) },</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10">
+      <c r="A160" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B159" s="2">
+      <c r="B160" s="2">
         <v>704</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="C160" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D160" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E160" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="F159" s="3">
-        <v>100</v>
-      </c>
-      <c r="G159" s="3">
+      <c r="F160" s="3">
+        <v>100</v>
+      </c>
+      <c r="G160" s="3">
         <v>0</v>
       </c>
-      <c r="H159" s="3" t="s">
+      <c r="H160" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="I159" s="3" t="str">
+      <c r="I160" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency VND { get; private set; }</v>
       </c>
-      <c r="J159" s="3" t="str">
+      <c r="J160" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{VND = new Currency("VND", 704, "Vietnamese Dong", 0)},</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10">
-      <c r="A160" s="2" t="s">
+        <v>{ VND = new Currency("VND", 704, "Vietnamese Dong", 0) },</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10">
+      <c r="A161" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B160" s="2">
+      <c r="B161" s="2">
         <v>548</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="C161" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="D161" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="F160" s="3">
+      <c r="F161" s="3">
         <v>1</v>
       </c>
-      <c r="G160" s="3">
+      <c r="G161" s="3">
         <v>0</v>
       </c>
-      <c r="H160" s="3" t="s">
+      <c r="H161" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="I160" s="3" t="str">
+      <c r="I161" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency VUV { get; private set; }</v>
       </c>
-      <c r="J160" s="3" t="str">
+      <c r="J161" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{VUV = new Currency("VUV", 548, "Vanuatu Vatu", 0)},</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10">
-      <c r="A161" s="2" t="s">
+        <v>{ VUV = new Currency("VUV", 548, "Vanuatu Vatu", 0) },</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
+      <c r="A162" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B161" s="2">
+      <c r="B162" s="2">
         <v>882</v>
       </c>
-      <c r="C161" s="3" t="s">
+      <c r="C162" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D162" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E161" s="3" t="s">
+      <c r="E162" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="F161" s="3">
-        <v>100</v>
-      </c>
-      <c r="G161" s="3">
-        <v>2</v>
-      </c>
-      <c r="H161" s="3" t="s">
+      <c r="F162" s="3">
+        <v>100</v>
+      </c>
+      <c r="G162" s="3">
+        <v>2</v>
+      </c>
+      <c r="H162" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="I161" s="3" t="str">
+      <c r="I162" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency WST { get; private set; }</v>
       </c>
-      <c r="J161" s="3" t="str">
+      <c r="J162" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{WST = new Currency("WST", 882, "Samoan Tala", 2)},</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10">
-      <c r="A162" s="2" t="s">
+        <v>{ WST = new Currency("WST", 882, "Samoan Tala", 2) },</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10">
+      <c r="A163" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B162" s="2">
+      <c r="B163" s="2">
         <v>950</v>
       </c>
-      <c r="C162" s="3" t="s">
+      <c r="C163" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="D162" s="3" t="s">
+      <c r="D163" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="E162" s="3" t="s">
+      <c r="E163" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="F162" s="3">
-        <v>100</v>
-      </c>
-      <c r="G162" s="3">
-        <v>2</v>
-      </c>
-      <c r="H162" s="3" t="s">
+      <c r="F163" s="3">
+        <v>100</v>
+      </c>
+      <c r="G163" s="3">
+        <v>2</v>
+      </c>
+      <c r="H163" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="I162" s="3" t="str">
+      <c r="I163" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XAF { get; private set; }</v>
       </c>
-      <c r="J162" s="3" t="str">
+      <c r="J163" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XAF = new Currency("XAF", 950, "Central African CFA Franc", 2)},</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10">
-      <c r="A163" s="2" t="s">
+        <v>{ XAF = new Currency("XAF", 950, "Central African CFA Franc", 2) },</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10">
+      <c r="A164" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B163" s="2">
+      <c r="B164" s="2">
         <v>961</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C164" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F163" s="3">
+      <c r="F164" s="3">
         <v>1</v>
       </c>
-      <c r="G163" s="3">
+      <c r="G164" s="3">
         <v>0</v>
       </c>
-      <c r="I163" s="3" t="str">
+      <c r="I164" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XAG { get; private set; }</v>
       </c>
-      <c r="J163" s="3" t="str">
+      <c r="J164" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XAG = new Currency("XAG", 961, "Silver", 0)},</v>
-      </c>
-    </row>
-    <row r="164" spans="1:10">
-      <c r="A164" s="2" t="s">
+        <v>{ XAG = new Currency("XAG", 961, "Silver", 0) },</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10">
+      <c r="A165" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B164" s="2">
+      <c r="B165" s="2">
         <v>959</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C165" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F164" s="3">
+      <c r="F165" s="3">
         <v>1</v>
       </c>
-      <c r="G164" s="3">
+      <c r="G165" s="3">
         <v>0</v>
       </c>
-      <c r="I164" s="3" t="str">
+      <c r="I165" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XAU { get; private set; }</v>
       </c>
-      <c r="J164" s="3" t="str">
+      <c r="J165" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XAU = new Currency("XAU", 959, "Gold", 0)},</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10">
-      <c r="A165" s="2" t="s">
+        <v>{ XAU = new Currency("XAU", 959, "Gold", 0) },</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10">
+      <c r="A166" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B165" s="2">
+      <c r="B166" s="2">
         <v>955</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="C166" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="F165" s="3">
+      <c r="F166" s="3">
         <v>1</v>
       </c>
-      <c r="G165" s="3">
+      <c r="G166" s="3">
         <v>0</v>
       </c>
-      <c r="I165" s="3" t="str">
+      <c r="I166" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XBA { get; private set; }</v>
       </c>
-      <c r="J165" s="3" t="str">
+      <c r="J166" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XBA = new Currency("XBA", 955, "Bond Markets Units European Composite Unit (EURCO)", 0)},</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10">
-      <c r="A166" s="2" t="s">
+        <v>{ XBA = new Currency("XBA", 955, "Bond Markets Units European Composite Unit (EURCO)", 0) },</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10">
+      <c r="A167" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B166" s="2">
+      <c r="B167" s="2">
         <v>956</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C167" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="F166" s="3">
+      <c r="F167" s="3">
         <v>1</v>
       </c>
-      <c r="G166" s="3">
+      <c r="G167" s="3">
         <v>0</v>
       </c>
-      <c r="I166" s="3" t="str">
+      <c r="I167" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XBB { get; private set; }</v>
       </c>
-      <c r="J166" s="3" t="str">
+      <c r="J167" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XBB = new Currency("XBB", 956, "European Monetary Unit (E.M.U.-6)", 0)},</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10">
-      <c r="A167" s="2" t="s">
+        <v>{ XBB = new Currency("XBB", 956, "European Monetary Unit (E.M.U.-6)", 0) },</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10">
+      <c r="A168" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B167" s="2">
+      <c r="B168" s="2">
         <v>957</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C168" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="F167" s="3">
+      <c r="F168" s="3">
         <v>1</v>
       </c>
-      <c r="G167" s="3">
+      <c r="G168" s="3">
         <v>0</v>
       </c>
-      <c r="I167" s="3" t="str">
+      <c r="I168" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XBC { get; private set; }</v>
       </c>
-      <c r="J167" s="3" t="str">
+      <c r="J168" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XBC = new Currency("XBC", 957, "European Unit of Account 9 (E.U.A.-9)", 0)},</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10">
-      <c r="A168" s="2" t="s">
+        <v>{ XBC = new Currency("XBC", 957, "European Unit of Account 9 (E.U.A.-9)", 0) },</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10">
+      <c r="A169" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B168" s="2">
+      <c r="B169" s="2">
         <v>958</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="C169" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="F168" s="3">
+      <c r="F169" s="3">
         <v>1</v>
       </c>
-      <c r="G168" s="3">
+      <c r="G169" s="3">
         <v>0</v>
       </c>
-      <c r="I168" s="3" t="str">
+      <c r="I169" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XBD { get; private set; }</v>
       </c>
-      <c r="J168" s="3" t="str">
+      <c r="J169" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XBD = new Currency("XBD", 958, "European Unit of Account 17 (E.U.A.-17)", 0)},</v>
-      </c>
-    </row>
-    <row r="169" spans="1:10">
-      <c r="A169" s="2" t="s">
+        <v>{ XBD = new Currency("XBD", 958, "European Unit of Account 17 (E.U.A.-17)", 0) },</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10">
+      <c r="A170" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B169" s="2">
+      <c r="B170" s="2">
         <v>951</v>
       </c>
-      <c r="C169" s="3" t="s">
+      <c r="C170" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D169" s="3" t="s">
+      <c r="D170" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="E169" s="3" t="s">
+      <c r="E170" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F169" s="3">
-        <v>100</v>
-      </c>
-      <c r="G169" s="3">
-        <v>2</v>
-      </c>
-      <c r="H169" s="3" t="s">
+      <c r="F170" s="3">
+        <v>100</v>
+      </c>
+      <c r="G170" s="3">
+        <v>2</v>
+      </c>
+      <c r="H170" s="3" t="s">
         <v>664</v>
       </c>
-      <c r="I169" s="3" t="str">
+      <c r="I170" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XCD { get; private set; }</v>
       </c>
-      <c r="J169" s="3" t="str">
+      <c r="J170" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XCD = new Currency("XCD", 951, "East Caribbean Dollar", 2)},</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10">
-      <c r="A170" s="2" t="s">
+        <v>{ XCD = new Currency("XCD", 951, "East Caribbean Dollar", 2) },</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10">
+      <c r="A171" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B170" s="2">
+      <c r="B171" s="2">
         <v>960</v>
       </c>
-      <c r="C170" s="3" t="s">
+      <c r="C171" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="F170" s="3">
+      <c r="F171" s="3">
         <v>1</v>
       </c>
-      <c r="G170" s="3">
+      <c r="G171" s="3">
         <v>0</v>
       </c>
-      <c r="I170" s="3" t="str">
+      <c r="I171" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XDR { get; private set; }</v>
       </c>
-      <c r="J170" s="3" t="str">
+      <c r="J171" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XDR = new Currency("XDR", 960, "SDR (IMF Special Drawing Rights)", 0)},</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10">
-      <c r="A171" s="2" t="s">
+        <v>{ XDR = new Currency("XDR", 960, "SDR (IMF Special Drawing Rights)", 0) },</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10">
+      <c r="A172" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B171" s="2">
+      <c r="B172" s="2">
         <v>0</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C172" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="F171" s="3">
+      <c r="F172" s="3">
         <v>1</v>
       </c>
-      <c r="G171" s="3">
+      <c r="G172" s="3">
         <v>0</v>
       </c>
-      <c r="I171" s="3" t="str">
+      <c r="I172" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XFU { get; private set; }</v>
       </c>
-      <c r="J171" s="3" t="str">
+      <c r="J172" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XFU = new Currency("XFU", 0, "UIC-Franc", 0)},</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10">
-      <c r="A172" s="2" t="s">
+        <v>{ XFU = new Currency("XFU", 0, "UIC-Franc", 0) },</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10">
+      <c r="A173" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B172" s="2">
+      <c r="B173" s="2">
         <v>952</v>
       </c>
-      <c r="C172" s="3" t="s">
+      <c r="C173" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="D172" s="3" t="s">
+      <c r="D173" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="E172" s="3" t="s">
+      <c r="E173" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="F172" s="3">
-        <v>100</v>
-      </c>
-      <c r="G172" s="3">
-        <v>2</v>
-      </c>
-      <c r="H172" s="3" t="s">
+      <c r="F173" s="3">
+        <v>100</v>
+      </c>
+      <c r="G173" s="3">
+        <v>2</v>
+      </c>
+      <c r="H173" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="I172" s="3" t="str">
+      <c r="I173" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XOF { get; private set; }</v>
       </c>
-      <c r="J172" s="3" t="str">
+      <c r="J173" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XOF = new Currency("XOF", 952, "West African CFA Franc", 2)},</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10">
-      <c r="A173" s="2" t="s">
+        <v>{ XOF = new Currency("XOF", 952, "West African CFA Franc", 2) },</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10">
+      <c r="A174" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B173" s="2">
+      <c r="B174" s="2">
         <v>964</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C174" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F173" s="3">
+      <c r="F174" s="3">
         <v>1</v>
       </c>
-      <c r="G173" s="3">
+      <c r="G174" s="3">
         <v>0</v>
       </c>
-      <c r="I173" s="3" t="str">
+      <c r="I174" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XPD { get; private set; }</v>
       </c>
-      <c r="J173" s="3" t="str">
+      <c r="J174" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XPD = new Currency("XPD", 964, "Palladium", 0)},</v>
-      </c>
-    </row>
-    <row r="174" spans="1:10">
-      <c r="A174" s="2" t="s">
+        <v>{ XPD = new Currency("XPD", 964, "Palladium", 0) },</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10">
+      <c r="A175" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B174" s="2">
+      <c r="B175" s="2">
         <v>953</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C175" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D174" s="3" t="s">
+      <c r="D175" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="E174" s="3" t="s">
+      <c r="E175" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="F174" s="3">
-        <v>100</v>
-      </c>
-      <c r="G174" s="3">
-        <v>2</v>
-      </c>
-      <c r="H174" s="3" t="s">
+      <c r="F175" s="3">
+        <v>100</v>
+      </c>
+      <c r="G175" s="3">
+        <v>2</v>
+      </c>
+      <c r="H175" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="I174" s="3" t="str">
+      <c r="I175" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XPF { get; private set; }</v>
       </c>
-      <c r="J174" s="3" t="str">
+      <c r="J175" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XPF = new Currency("XPF", 953, "CFP Franc", 2)},</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10">
-      <c r="A175" s="2" t="s">
+        <v>{ XPF = new Currency("XPF", 953, "CFP Franc", 2) },</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10">
+      <c r="A176" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B175" s="2">
+      <c r="B176" s="2">
         <v>962</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C176" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="F175" s="3">
+      <c r="F176" s="3">
         <v>1</v>
       </c>
-      <c r="G175" s="3">
+      <c r="G176" s="3">
         <v>0</v>
       </c>
-      <c r="I175" s="3" t="str">
+      <c r="I176" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XPT { get; private set; }</v>
       </c>
-      <c r="J175" s="3" t="str">
+      <c r="J176" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XPT = new Currency("XPT", 962, "Platinum", 0)},</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10">
-      <c r="A176" s="2" t="s">
+        <v>{ XPT = new Currency("XPT", 962, "Platinum", 0) },</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10">
+      <c r="A177" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B176" s="2">
+      <c r="B177" s="2">
         <v>963</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C177" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F176" s="3">
+      <c r="F177" s="3">
         <v>1</v>
       </c>
-      <c r="G176" s="3">
+      <c r="G177" s="3">
         <v>0</v>
       </c>
-      <c r="I176" s="3" t="str">
+      <c r="I177" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XTS { get; private set; }</v>
       </c>
-      <c r="J176" s="3" t="str">
+      <c r="J177" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XTS = new Currency("XTS", 963, "Codes specifically reserved for testing purposes", 0)},</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10">
-      <c r="A177" s="2" t="s">
+        <v>{ XTS = new Currency("XTS", 963, "Codes specifically reserved for testing purposes", 0) },</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10">
+      <c r="A178" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B177" s="2">
+      <c r="B178" s="2">
         <v>999</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C178" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="F177" s="3">
+      <c r="F178" s="3">
         <v>1</v>
       </c>
-      <c r="G177" s="3">
+      <c r="G178" s="3">
         <v>0</v>
       </c>
-      <c r="I177" s="3" t="str">
+      <c r="I178" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency XXX { get; private set; }</v>
       </c>
-      <c r="J177" s="3" t="str">
+      <c r="J178" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{XXX = new Currency("XXX", 999, "Transactions without currency", 0)},</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10">
-      <c r="A178" s="2" t="s">
+        <v>{ XXX = new Currency("XXX", 999, "Transactions without currency", 0) },</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10">
+      <c r="A179" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B178" s="2">
+      <c r="B179" s="2">
         <v>886</v>
       </c>
-      <c r="C178" s="3" t="s">
+      <c r="C179" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="D178" s="3" t="s">
+      <c r="D179" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="E178" s="3" t="s">
+      <c r="E179" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="F178" s="3">
-        <v>100</v>
-      </c>
-      <c r="G178" s="3">
-        <v>2</v>
-      </c>
-      <c r="I178" s="3" t="str">
+      <c r="F179" s="3">
+        <v>100</v>
+      </c>
+      <c r="G179" s="3">
+        <v>2</v>
+      </c>
+      <c r="I179" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency YER { get; private set; }</v>
       </c>
-      <c r="J178" s="3" t="str">
+      <c r="J179" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{YER = new Currency("YER", 886, "Yemeni Rial", 2)},</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10">
-      <c r="A179" s="2" t="s">
+        <v>{ YER = new Currency("YER", 886, "Yemeni Rial", 2) },</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10">
+      <c r="A180" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B179" s="2">
+      <c r="B180" s="2">
         <v>710</v>
       </c>
-      <c r="C179" s="3" t="s">
+      <c r="C180" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="D179" s="3" t="s">
+      <c r="D180" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E179" s="3" t="s">
+      <c r="E180" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F179" s="3">
-        <v>100</v>
-      </c>
-      <c r="G179" s="3">
-        <v>2</v>
-      </c>
-      <c r="H179" s="3" t="s">
+      <c r="F180" s="3">
+        <v>100</v>
+      </c>
+      <c r="G180" s="3">
+        <v>2</v>
+      </c>
+      <c r="H180" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="I179" s="3" t="str">
+      <c r="I180" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency ZAR { get; private set; }</v>
       </c>
-      <c r="J179" s="3" t="str">
+      <c r="J180" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{ZAR = new Currency("ZAR", 710, "South African Rand", 2)},</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10">
-      <c r="A180" s="2" t="s">
+        <v>{ ZAR = new Currency("ZAR", 710, "South African Rand", 2) },</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10">
+      <c r="A181" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B180" s="2">
+      <c r="B181" s="2">
         <v>894</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="C181" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D180" s="3" t="s">
+      <c r="D181" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E180" s="3" t="s">
+      <c r="E181" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="F180" s="3">
-        <v>100</v>
-      </c>
-      <c r="G180" s="3">
-        <v>2</v>
-      </c>
-      <c r="H180" s="3" t="s">
+      <c r="F181" s="3">
+        <v>100</v>
+      </c>
+      <c r="G181" s="3">
+        <v>2</v>
+      </c>
+      <c r="H181" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="I180" s="3" t="str">
+      <c r="I181" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency ZMK { get; private set; }</v>
       </c>
-      <c r="J180" s="3" t="str">
+      <c r="J181" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{ZMK = new Currency("ZMK", 894, "Zambian Kwacha", 2)},</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10">
-      <c r="A181" s="2" t="s">
+        <v>{ ZMK = new Currency("ZMK", 894, "Zambian Kwacha", 2) },</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10">
+      <c r="A182" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B181" s="2">
+      <c r="B182" s="2">
         <v>932</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C182" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D181" s="3" t="s">
+      <c r="D182" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="E181" s="3" t="s">
+      <c r="E182" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F181" s="3">
-        <v>100</v>
-      </c>
-      <c r="G181" s="3">
-        <v>2</v>
-      </c>
-      <c r="H181" s="3" t="s">
+      <c r="F182" s="3">
+        <v>100</v>
+      </c>
+      <c r="G182" s="3">
+        <v>2</v>
+      </c>
+      <c r="H182" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="I181" s="3" t="str">
+      <c r="I182" s="8" t="str">
         <f t="shared" si="4"/>
         <v>public static Currency ZWL { get; private set; }</v>
       </c>
-      <c r="J181" s="3" t="str">
+      <c r="J182" s="8" t="str">
         <f t="shared" si="5"/>
-        <v>{ZWL = new Currency("ZWL", 932, "Zimbabwe Dollar", 2)},</v>
+        <v>{ ZWL = new Currency("ZWL", 932, "Zimbabwe Dollar", 2) },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>